<commit_message>
Finished testing methods for resize
</commit_message>
<xml_diff>
--- a/detect_methods_comp.xlsx
+++ b/detect_methods_comp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iwaya\Escritorio\Code\FaceRecogServer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F129B7-8A1E-4702-B78A-E785D29A3323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC94E1A-5409-4937-B925-E4F457A36B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="get_frontal_face_detector()" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="28">
   <si>
     <t>Up Sampling [dlib.get_frontal_face_detector()]</t>
   </si>
@@ -102,6 +102,27 @@
   <si>
     <t>N/A</t>
   </si>
+  <si>
+    <t>test_348_300_crop.mp4 (348, 300)px</t>
+  </si>
+  <si>
+    <t>Total: ~1:21m</t>
+  </si>
+  <si>
+    <t>4m</t>
+  </si>
+  <si>
+    <t>3m</t>
+  </si>
+  <si>
+    <t>2m</t>
+  </si>
+  <si>
+    <t>1m</t>
+  </si>
+  <si>
+    <t>DNN SR</t>
+  </si>
 </sst>
 </file>
 
@@ -124,7 +145,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,6 +167,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -204,9 +231,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -225,10 +249,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -857,6 +884,640 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Rendimiento de dib.get_frontal_face_detector()</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.764414512629525E-2"/>
+          <c:y val="0.1647071452598394"/>
+          <c:w val="0.8870541933270456"/>
+          <c:h val="0.67675822744305369"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.9315862953189569E-2"/>
+                  <c:y val="-4.6236472651544035E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-1591-44FF-BAAB-DB420C5C67BF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.8072621748300712E-2"/>
+                  <c:y val="-4.6236472651543896E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-1591-44FF-BAAB-DB420C5C67BF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.0349256193294611E-2"/>
+                  <c:y val="-4.9937605314709935E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-1591-44FF-BAAB-DB420C5C67BF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.8113425201810398E-2"/>
+                  <c:y val="-4.6236472651544035E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-1591-44FF-BAAB-DB420C5C67BF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'get_frontal_face_detector()'!$H$3:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'get_frontal_face_detector()'!$N$3:$N$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.6351666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.4816666666666665</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.9415</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>61.233500000000006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>241.39249999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>983.61500000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1591-44FF-BAAB-DB420C5C67BF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="656830976"/>
+        <c:axId val="651988608"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="656830976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Número</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> de upsamples</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="651988608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="651988608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Tiempo</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> [m]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="5.5640163990859446E-3"/>
+              <c:y val="0.40492285615533324"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="656830976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
               <a:rPr lang="en-US"/>
               <a:t>Rendimiento</a:t>
             </a:r>
@@ -1242,6 +1903,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.3168724279835391E-2"/>
+              <c:y val="0.36517108479169691"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1271,7 +1940,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1357,7 +2026,544 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Rendimiento del método Resize de OpenCV</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Resize (OpenCV)'!$H$3:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Resize (OpenCV)'!$N$3:$N$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.5919999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.3691666666666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.5018333333333338</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.656166666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22.458833333333335</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.197333333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E684-4C5A-BF60-DEAD2C4ECBEE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="693463104"/>
+        <c:axId val="651993568"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="693463104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Factor</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> de resize</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="651993568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="651993568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Tiempo</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> [m]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.6243654822335026E-2"/>
+              <c:y val="0.36560886188508612"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="693463104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1459,6 +2665,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'DeepNeuralNetworks Methods'!$A$6:$A$8</c:f>
@@ -1501,8 +2765,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1713,7 +2978,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1745,6 +3010,509 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1109140607"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Comparación entre métodos SR</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'DeepNeuralNetworks Methods'!$G$6:$G$8</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>ESPCN_x4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FSRCNN_x4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>LapSRN_x4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'DeepNeuralNetworks Methods'!$M$6:$M$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>21.753166666666669</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27.911000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200.411</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DAA6-4B2A-AA16-15E6B3BD7913}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="856541920"/>
+        <c:axId val="659510640"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="856541920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Método</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="659510640"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="659510640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Tiempo</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> [m]</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="856541920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1913,6 +3681,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2946,6 +4834,1543 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3461,9 +6886,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1590261</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>177096</xdr:rowOff>
+      <xdr:colOff>1031875</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3490,6 +6915,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>611185</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>188119</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>595313</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EE31B95-B077-3769-AE27-C828BF66B8A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3504,9 +6965,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1592790</xdr:colOff>
+      <xdr:colOff>1039812</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:rowOff>182563</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3526,6 +6987,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>7937</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>188119</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>7937</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>182563</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DE63D3E-C853-B265-98D4-53D9D2817529}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3567,6 +7064,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>180181</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>309563</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>65881</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81FD001C-C027-4BF1-8C1E-D0CEE379AABE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3838,23 +7371,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.54296875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="44.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -3864,32 +7404,62 @@
       <c r="C1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="H1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>10</v>
       </c>
+      <c r="H2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="7">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -3898,20 +7468,46 @@
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>37.4</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <f>D3/60</f>
         <v>0.62333333333333329</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="8">
         <f>1</f>
         <v>1</v>
       </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="5">
+        <v>98.11</v>
+      </c>
+      <c r="N3" s="5">
+        <f>M3/60</f>
+        <v>1.6351666666666667</v>
+      </c>
+      <c r="O3" s="8">
+        <f>M3/81</f>
+        <v>1.2112345679012346</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="7">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -3920,20 +7516,46 @@
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>76.239999999999995</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <f t="shared" ref="E4:E8" si="0">D4/60</f>
         <v>1.2706666666666666</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="8">
         <f>E4/E3</f>
         <v>2.0385026737967915</v>
       </c>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="5">
+        <v>268.89999999999998</v>
+      </c>
+      <c r="N4" s="5">
+        <f>M4/60</f>
+        <v>4.4816666666666665</v>
+      </c>
+      <c r="O4" s="8">
+        <f t="shared" ref="O4:O7" si="1">M4/81</f>
+        <v>3.3197530864197526</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="7">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -3942,20 +7564,46 @@
       <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>191.54</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <f t="shared" si="0"/>
         <v>3.192333333333333</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="8">
         <f>E5/E3</f>
         <v>5.1213903743315505</v>
       </c>
+      <c r="H5" s="2">
+        <v>2</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" s="5">
+        <v>956.49</v>
+      </c>
+      <c r="N5" s="5">
+        <f>M5/60</f>
+        <v>15.9415</v>
+      </c>
+      <c r="O5" s="8">
+        <f t="shared" si="1"/>
+        <v>11.808518518518518</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="7">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -3964,20 +7612,46 @@
       <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>419.84</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <f t="shared" si="0"/>
         <v>6.9973333333333327</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="8">
         <f>E6/E3</f>
         <v>11.22566844919786</v>
       </c>
+      <c r="H6" s="2">
+        <v>3</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="5">
+        <v>3674.01</v>
+      </c>
+      <c r="N6" s="5">
+        <f>M6/60</f>
+        <v>61.233500000000006</v>
+      </c>
+      <c r="O6" s="8">
+        <f t="shared" si="1"/>
+        <v>45.358148148148153</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="8">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -3986,20 +7660,46 @@
       <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>1559.89</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <f t="shared" si="0"/>
         <v>25.99816666666667</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="8">
         <f>E7/E3</f>
         <v>41.708288770053485</v>
       </c>
+      <c r="H7" s="2">
+        <v>4</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M7" s="5">
+        <v>14483.55</v>
+      </c>
+      <c r="N7" s="5">
+        <f>M7/60</f>
+        <v>241.39249999999998</v>
+      </c>
+      <c r="O7" s="8">
+        <f>M7/81</f>
+        <v>178.80925925925925</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="7">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -4008,47 +7708,58 @@
       <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>5878.92</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <f t="shared" si="0"/>
         <v>97.981999999999999</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="8">
         <f>E8/E3</f>
         <v>157.1903743315508</v>
       </c>
+      <c r="H8" s="2">
+        <v>5</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M8" s="5">
+        <v>59016.9</v>
+      </c>
+      <c r="N8" s="5">
+        <f>M8/60</f>
+        <v>983.61500000000001</v>
+      </c>
+      <c r="O8" s="8">
+        <f>M8/81</f>
+        <v>728.60370370370367</v>
+      </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4058,23 +7769,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6706964-F93E-4934-BEB2-8D6878ECF54C}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7265625" customWidth="1"/>
-    <col min="3" max="3" width="23.6328125" customWidth="1"/>
-    <col min="4" max="4" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.36328125" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -4084,34 +7800,70 @@
       <c r="C1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
+      <c r="H1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>10</v>
       </c>
+      <c r="H2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="7">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -4120,20 +7872,46 @@
       <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>37.93</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <f>D3/60</f>
         <v>0.63216666666666665</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="8">
         <f>1</f>
         <v>1</v>
       </c>
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="2">
+        <v>95.52</v>
+      </c>
+      <c r="N3" s="5">
+        <f>M3/60</f>
+        <v>1.5919999999999999</v>
+      </c>
+      <c r="O3" s="8">
+        <f>M3/81</f>
+        <v>1.1792592592592592</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="7">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -4142,20 +7920,46 @@
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>42.94</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <f t="shared" ref="E4:E8" si="0">D4/60</f>
         <v>0.71566666666666667</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="8">
         <f>E4/E3</f>
         <v>1.1320854205114685</v>
       </c>
+      <c r="H4" s="2">
+        <v>2</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2">
+        <v>262.14999999999998</v>
+      </c>
+      <c r="N4" s="5">
+        <f>M4/60</f>
+        <v>4.3691666666666666</v>
+      </c>
+      <c r="O4" s="8">
+        <f>M4/81</f>
+        <v>3.2364197530864196</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="7">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -4164,20 +7968,46 @@
       <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>75.97</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <f t="shared" si="0"/>
         <v>1.2661666666666667</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="8">
         <f>E5/E3</f>
         <v>2.0029000790930662</v>
       </c>
+      <c r="H5" s="2">
+        <v>3</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" s="2">
+        <v>510.11</v>
+      </c>
+      <c r="N5" s="5">
+        <f>M5/60</f>
+        <v>8.5018333333333338</v>
+      </c>
+      <c r="O5" s="8">
+        <f>M5/81</f>
+        <v>6.2976543209876548</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="7">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -4186,20 +8016,46 @@
       <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>113.31</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <f t="shared" si="0"/>
         <v>1.8885000000000001</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="8">
         <f>E6/E3</f>
         <v>2.9873451094120749</v>
       </c>
+      <c r="H6" s="2">
+        <v>4</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="2">
+        <v>879.37</v>
+      </c>
+      <c r="N6" s="5">
+        <f>M6/60</f>
+        <v>14.656166666666667</v>
+      </c>
+      <c r="O6" s="8">
+        <f>M6/81</f>
+        <v>10.856419753086421</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="7">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -4208,20 +8064,46 @@
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>154.19999999999999</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <f t="shared" si="0"/>
         <v>2.57</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="8">
         <f>E7/E3</f>
         <v>4.0653836013709466</v>
       </c>
+      <c r="H7" s="2">
+        <v>5</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M7" s="2">
+        <v>1347.53</v>
+      </c>
+      <c r="N7" s="5">
+        <f>M7/60</f>
+        <v>22.458833333333335</v>
+      </c>
+      <c r="O7" s="8">
+        <f>M7/81</f>
+        <v>16.636172839506173</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="7">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -4230,16 +8112,42 @@
       <c r="C8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>198.09</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <f t="shared" si="0"/>
         <v>3.3014999999999999</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="8">
         <f>E8/E3</f>
         <v>5.2225151595043497</v>
+      </c>
+      <c r="H8" s="2">
+        <v>6</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M8" s="2">
+        <v>1931.84</v>
+      </c>
+      <c r="N8" s="5">
+        <f>M8/60</f>
+        <v>32.197333333333333</v>
+      </c>
+      <c r="O8" s="8">
+        <f>M8/81</f>
+        <v>23.849876543209877</v>
       </c>
     </row>
   </sheetData>
@@ -4250,23 +8158,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EDFC79-1BF5-4D0E-ADD4-A69D2D4846CD}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -4276,32 +8188,64 @@
       <c r="C1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
+      <c r="G1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="10" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="12"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -4310,16 +8254,37 @@
       <c r="C3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="13"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -4328,16 +8293,37 @@
       <c r="C4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="13"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -4346,16 +8332,37 @@
       <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="13"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -4364,17 +8371,39 @@
       <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>152.66999999999999</v>
       </c>
-      <c r="E6" s="6">
-        <f t="shared" ref="E4:E8" si="0">D6/60</f>
+      <c r="E6" s="5">
+        <f t="shared" ref="E6:E8" si="0">D6/60</f>
         <v>2.5444999999999998</v>
       </c>
-      <c r="F6" s="13"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1305.19</v>
+      </c>
+      <c r="M6" s="5">
+        <f>L6/60</f>
+        <v>21.753166666666669</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -4383,17 +8412,39 @@
       <c r="C7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>152.69</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <f t="shared" si="0"/>
         <v>2.5448333333333335</v>
       </c>
-      <c r="F7" s="13"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L7" s="2">
+        <v>1674.66</v>
+      </c>
+      <c r="M7" s="5">
+        <f>L7/60</f>
+        <v>27.911000000000001</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -4402,14 +8453,36 @@
       <c r="C8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>1212.56</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <f t="shared" si="0"/>
         <v>20.209333333333333</v>
       </c>
-      <c r="F8" s="13"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L8" s="5">
+        <v>12024.66</v>
+      </c>
+      <c r="M8" s="5">
+        <f>L8/60</f>
+        <v>200.411</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added new models and support to send and get embeddings from DB
</commit_message>
<xml_diff>
--- a/detect_methods_comp.xlsx
+++ b/detect_methods_comp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iwaya\Escritorio\Code\FaceRecogServer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E6C7C1-0054-4851-B291-5C5DED862C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF01934F-C8A2-4DFD-8C1D-30A40352A040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resize (OpenCV)" sheetId="2" r:id="rId1"/>
@@ -521,7 +521,25 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -530,43 +548,40 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -581,40 +596,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -7732,7 +7732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6706964-F93E-4934-BEB2-8D6878ECF54C}">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="103" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -8767,15 +8767,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB5E59B-51C7-438E-AB32-5EE19B87C996}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="130" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26:H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.6328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.90625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7265625" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.453125" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.7265625" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.81640625" style="14" customWidth="1"/>
@@ -8786,1022 +8786,957 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="52" t="s">
+      <c r="C1" s="35"/>
+      <c r="D1" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="51"/>
-      <c r="G1" s="52" t="s">
+      <c r="F1" s="35"/>
+      <c r="G1" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="53" t="s">
+      <c r="H1" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="51"/>
-      <c r="J1" s="52" t="s">
+      <c r="I1" s="35"/>
+      <c r="J1" s="25" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="37" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="16">
         <v>1.2</v>
       </c>
-      <c r="C2" s="49">
+      <c r="C2" s="40">
         <v>1</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="E2" s="37" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="16">
         <v>1.5</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="46" t="s">
+      <c r="H2" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="49">
+      <c r="I2" s="40">
         <v>1</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="J2" s="26" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="47"/>
+      <c r="A3" s="38"/>
       <c r="B3" s="15">
         <v>1.5</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="47"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="38"/>
       <c r="F3" s="15">
         <v>2</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="30"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="27"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="47"/>
+      <c r="A4" s="38"/>
       <c r="B4" s="15">
         <v>1.7</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="47"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="15">
         <v>2.5</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="38">
+      <c r="G4" s="27"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="41">
         <v>2</v>
       </c>
-      <c r="J4" s="30"/>
+      <c r="J4" s="27"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="47"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="15">
         <v>2</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="47"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="38"/>
       <c r="F5" s="15">
         <v>3</v>
       </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="30"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="27"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="47"/>
+      <c r="A6" s="38"/>
       <c r="B6" s="15">
         <v>2.5</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="44" t="s">
+      <c r="C6" s="41"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="39" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="15">
         <v>1.5</v>
       </c>
-      <c r="G6" s="30"/>
-      <c r="H6" s="44" t="s">
+      <c r="G6" s="27"/>
+      <c r="H6" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="38">
+      <c r="I6" s="41">
         <v>1</v>
       </c>
-      <c r="J6" s="30"/>
+      <c r="J6" s="27"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="47"/>
+      <c r="A7" s="38"/>
       <c r="B7" s="15">
         <v>3</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="44"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="39"/>
       <c r="F7" s="15">
         <v>2</v>
       </c>
-      <c r="G7" s="30"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="30"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="27"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="47"/>
+      <c r="A8" s="38"/>
       <c r="B8" s="15">
         <v>1.2</v>
       </c>
-      <c r="C8" s="38">
+      <c r="C8" s="41">
         <v>2</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="44"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="39"/>
       <c r="F8" s="15">
         <v>2.5</v>
       </c>
-      <c r="G8" s="30"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="38">
+      <c r="G8" s="27"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="41">
         <v>2</v>
       </c>
-      <c r="J8" s="30"/>
+      <c r="J8" s="27"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="47"/>
+      <c r="A9" s="38"/>
       <c r="B9" s="15">
         <v>1.5</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="44"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="39"/>
       <c r="F9" s="15">
         <v>3</v>
       </c>
-      <c r="G9" s="30"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="30"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="27"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="47"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="15">
         <v>1.7</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="44" t="s">
+      <c r="C10" s="41"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="39" t="s">
         <v>15</v>
       </c>
       <c r="F10" s="15">
         <v>1.5</v>
       </c>
-      <c r="G10" s="30"/>
-      <c r="H10" s="44" t="s">
+      <c r="G10" s="27"/>
+      <c r="H10" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="38">
+      <c r="I10" s="41">
         <v>1</v>
       </c>
-      <c r="J10" s="30"/>
+      <c r="J10" s="27"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="47"/>
+      <c r="A11" s="38"/>
       <c r="B11" s="15">
         <v>2</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="44"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="39"/>
       <c r="F11" s="15">
         <v>2</v>
       </c>
-      <c r="G11" s="30"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="30"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="27"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="47"/>
+      <c r="A12" s="38"/>
       <c r="B12" s="15">
         <v>2.5</v>
       </c>
-      <c r="C12" s="38"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="44"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="15">
         <v>2.5</v>
       </c>
-      <c r="G12" s="30"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="38">
+      <c r="G12" s="27"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="41">
         <v>2</v>
       </c>
-      <c r="J12" s="30"/>
+      <c r="J12" s="27"/>
     </row>
     <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="48"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="17">
         <v>3</v>
       </c>
-      <c r="C13" s="39"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="45"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="44"/>
       <c r="F13" s="17">
         <v>3</v>
       </c>
-      <c r="G13" s="34"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="34"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="28"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="45" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="18">
         <v>1.2</v>
       </c>
-      <c r="C14" s="43">
+      <c r="C14" s="48">
         <v>1</v>
       </c>
-      <c r="D14" s="27" t="s">
+      <c r="D14" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="40" t="s">
+      <c r="E14" s="45" t="s">
         <v>13</v>
       </c>
       <c r="F14" s="18">
         <v>1.5</v>
       </c>
-      <c r="G14" s="29" t="s">
+      <c r="G14" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="H14" s="40" t="s">
+      <c r="H14" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="43">
+      <c r="I14" s="48">
         <v>1</v>
       </c>
-      <c r="J14" s="29" t="s">
+      <c r="J14" s="26" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="41"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="2">
         <v>1.5</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="41"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="46"/>
       <c r="F15" s="2">
         <v>2</v>
       </c>
-      <c r="G15" s="30"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="30"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="27"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="41"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="2">
         <v>1.7</v>
       </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="41"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="46"/>
       <c r="F16" s="2">
         <v>2.5</v>
       </c>
-      <c r="G16" s="30"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="32">
+      <c r="G16" s="27"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="49">
         <v>2</v>
       </c>
-      <c r="J16" s="30"/>
+      <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="41"/>
+      <c r="A17" s="46"/>
       <c r="B17" s="2">
         <v>2</v>
       </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="41"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="46"/>
       <c r="F17" s="2">
         <v>3</v>
       </c>
-      <c r="G17" s="30"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="30"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="27"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="41"/>
+      <c r="A18" s="46"/>
       <c r="B18" s="2">
         <v>2.5</v>
       </c>
-      <c r="C18" s="32"/>
-      <c r="D18" s="35" t="s">
+      <c r="C18" s="49"/>
+      <c r="D18" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="36" t="s">
+      <c r="E18" s="50" t="s">
         <v>14</v>
       </c>
       <c r="F18" s="2">
         <v>1.5</v>
       </c>
-      <c r="G18" s="30"/>
-      <c r="H18" s="36" t="s">
+      <c r="G18" s="27"/>
+      <c r="H18" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="I18" s="32">
+      <c r="I18" s="49">
         <v>1</v>
       </c>
-      <c r="J18" s="30"/>
+      <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="41"/>
+      <c r="A19" s="46"/>
       <c r="B19" s="2">
         <v>3</v>
       </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="36"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="50"/>
       <c r="F19" s="2">
         <v>2</v>
       </c>
-      <c r="G19" s="30"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="30"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="27"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="41"/>
+      <c r="A20" s="46"/>
       <c r="B20" s="2">
         <v>1.2</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="49">
         <v>2</v>
       </c>
       <c r="D20" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="36"/>
+      <c r="E20" s="50"/>
       <c r="F20" s="2">
         <v>2.5</v>
       </c>
-      <c r="G20" s="30"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="32">
+      <c r="G20" s="27"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="49">
         <v>2</v>
       </c>
-      <c r="J20" s="30"/>
+      <c r="J20" s="27"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" s="41"/>
+      <c r="A21" s="46"/>
       <c r="B21" s="2">
         <v>1.5</v>
       </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="35" t="s">
+      <c r="C21" s="49"/>
+      <c r="D21" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="36"/>
+      <c r="E21" s="50"/>
       <c r="F21" s="2">
         <v>3</v>
       </c>
-      <c r="G21" s="30"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="30"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="50"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="27"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="41"/>
+      <c r="A22" s="46"/>
       <c r="B22" s="2">
         <v>1.7</v>
       </c>
-      <c r="C22" s="32"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="36" t="s">
+      <c r="C22" s="49"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="50" t="s">
         <v>15</v>
       </c>
       <c r="F22" s="2">
         <v>1.5</v>
       </c>
-      <c r="G22" s="30"/>
-      <c r="H22" s="36" t="s">
+      <c r="G22" s="27"/>
+      <c r="H22" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="I22" s="32">
+      <c r="I22" s="49">
         <v>1</v>
       </c>
-      <c r="J22" s="30"/>
+      <c r="J22" s="27"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="41"/>
+      <c r="A23" s="46"/>
       <c r="B23" s="2">
         <v>2</v>
       </c>
-      <c r="C23" s="32"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="36"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="50"/>
       <c r="F23" s="2">
         <v>2</v>
       </c>
-      <c r="G23" s="30"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="30"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="27"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" s="41"/>
+      <c r="A24" s="46"/>
       <c r="B24" s="2">
         <v>2.5</v>
       </c>
-      <c r="C24" s="32"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="36"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="50"/>
       <c r="F24" s="2">
         <v>2.5</v>
       </c>
-      <c r="G24" s="30"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="32">
+      <c r="G24" s="27"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="49">
         <v>2</v>
       </c>
-      <c r="J24" s="30"/>
+      <c r="J24" s="27"/>
     </row>
     <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="42"/>
+      <c r="A25" s="47"/>
       <c r="B25" s="20">
         <v>3</v>
       </c>
-      <c r="C25" s="33"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="37"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="52"/>
       <c r="F25" s="20">
         <v>3</v>
       </c>
-      <c r="G25" s="34"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="34"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="51"/>
+      <c r="J25" s="28"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A26" s="46" t="s">
+      <c r="A26" s="37" t="s">
         <v>18</v>
       </c>
       <c r="B26" s="16">
         <v>1.2</v>
       </c>
-      <c r="C26" s="49">
+      <c r="C26" s="40">
         <v>1</v>
       </c>
-      <c r="D26" s="27" t="s">
+      <c r="D26" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="46" t="s">
+      <c r="E26" s="37" t="s">
         <v>13</v>
       </c>
       <c r="F26" s="16">
         <v>1.5</v>
       </c>
-      <c r="G26" s="27" t="s">
+      <c r="G26" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="H26" s="46" t="s">
+      <c r="H26" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="I26" s="49">
+      <c r="I26" s="40">
         <v>1</v>
       </c>
-      <c r="J26" s="29" t="s">
+      <c r="J26" s="26" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A27" s="47"/>
+      <c r="A27" s="38"/>
       <c r="B27" s="15">
         <v>1.5</v>
       </c>
-      <c r="C27" s="38"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="47"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="38"/>
       <c r="F27" s="15">
         <v>2</v>
       </c>
-      <c r="G27" s="25"/>
-      <c r="H27" s="47"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="30"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="27"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A28" s="47"/>
+      <c r="A28" s="38"/>
       <c r="B28" s="15">
         <v>1.7</v>
       </c>
-      <c r="C28" s="38"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="47"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="38"/>
       <c r="F28" s="15">
         <v>2.5</v>
       </c>
-      <c r="G28" s="25"/>
-      <c r="H28" s="47"/>
-      <c r="I28" s="38">
+      <c r="G28" s="31"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="41">
         <v>2</v>
       </c>
-      <c r="J28" s="30"/>
+      <c r="J28" s="27"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A29" s="47"/>
+      <c r="A29" s="38"/>
       <c r="B29" s="15">
         <v>2</v>
       </c>
-      <c r="C29" s="38"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="47"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="38"/>
       <c r="F29" s="15">
         <v>3</v>
       </c>
-      <c r="G29" s="25"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="30"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A30" s="47"/>
+      <c r="A30" s="38"/>
       <c r="B30" s="15">
         <v>2.5</v>
       </c>
-      <c r="C30" s="38"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="44" t="s">
+      <c r="C30" s="41"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="39" t="s">
         <v>14</v>
       </c>
       <c r="F30" s="15">
         <v>1.5</v>
       </c>
-      <c r="G30" s="26"/>
-      <c r="H30" s="44" t="s">
+      <c r="G30" s="32"/>
+      <c r="H30" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="I30" s="38">
+      <c r="I30" s="41">
         <v>1</v>
       </c>
-      <c r="J30" s="30"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A31" s="47"/>
+      <c r="A31" s="38"/>
       <c r="B31" s="15">
         <v>3</v>
       </c>
-      <c r="C31" s="38"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="44"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="39"/>
       <c r="F31" s="15">
         <v>2</v>
       </c>
       <c r="G31" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="H31" s="44"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="30"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="27"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A32" s="47"/>
+      <c r="A32" s="38"/>
       <c r="B32" s="15">
         <v>1.2</v>
       </c>
-      <c r="C32" s="38">
+      <c r="C32" s="41">
         <v>2</v>
       </c>
-      <c r="D32" s="25"/>
-      <c r="E32" s="44"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="39"/>
       <c r="F32" s="15">
         <v>2.5</v>
       </c>
-      <c r="G32" s="24" t="s">
+      <c r="G32" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="H32" s="44"/>
-      <c r="I32" s="38">
+      <c r="H32" s="39"/>
+      <c r="I32" s="41">
         <v>2</v>
       </c>
-      <c r="J32" s="30"/>
+      <c r="J32" s="27"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A33" s="47"/>
+      <c r="A33" s="38"/>
       <c r="B33" s="15">
         <v>1.5</v>
       </c>
-      <c r="C33" s="38"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="44"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="39"/>
       <c r="F33" s="15">
         <v>3</v>
       </c>
-      <c r="G33" s="25"/>
-      <c r="H33" s="44"/>
-      <c r="I33" s="38"/>
-      <c r="J33" s="30"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="41"/>
+      <c r="J33" s="27"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A34" s="47"/>
+      <c r="A34" s="38"/>
       <c r="B34" s="15">
         <v>1.7</v>
       </c>
-      <c r="C34" s="38"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="44" t="s">
+      <c r="C34" s="41"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="39" t="s">
         <v>15</v>
       </c>
       <c r="F34" s="15">
         <v>1.5</v>
       </c>
-      <c r="G34" s="25"/>
-      <c r="H34" s="44" t="s">
+      <c r="G34" s="31"/>
+      <c r="H34" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="I34" s="38">
+      <c r="I34" s="41">
         <v>1</v>
       </c>
-      <c r="J34" s="30"/>
+      <c r="J34" s="27"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A35" s="47"/>
+      <c r="A35" s="38"/>
       <c r="B35" s="15">
         <v>2</v>
       </c>
-      <c r="C35" s="38"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="44"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="39"/>
       <c r="F35" s="15">
         <v>2</v>
       </c>
-      <c r="G35" s="25"/>
-      <c r="H35" s="44"/>
-      <c r="I35" s="38"/>
-      <c r="J35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="39"/>
+      <c r="I35" s="41"/>
+      <c r="J35" s="29"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A36" s="47"/>
+      <c r="A36" s="38"/>
       <c r="B36" s="15">
         <v>2.5</v>
       </c>
-      <c r="C36" s="38"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="44"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="39"/>
       <c r="F36" s="15">
         <v>2.5</v>
       </c>
-      <c r="G36" s="25"/>
-      <c r="H36" s="44"/>
-      <c r="I36" s="38">
+      <c r="G36" s="31"/>
+      <c r="H36" s="39"/>
+      <c r="I36" s="41">
         <v>2</v>
       </c>
-      <c r="J36" s="54" t="s">
+      <c r="J36" s="53" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="48"/>
+      <c r="A37" s="42"/>
       <c r="B37" s="17">
         <v>3</v>
       </c>
-      <c r="C37" s="39"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="45"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="44"/>
       <c r="F37" s="17">
         <v>3</v>
       </c>
-      <c r="G37" s="28"/>
-      <c r="H37" s="45"/>
-      <c r="I37" s="39"/>
-      <c r="J37" s="55"/>
+      <c r="G37" s="34"/>
+      <c r="H37" s="44"/>
+      <c r="I37" s="43"/>
+      <c r="J37" s="54"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A38" s="40" t="s">
+      <c r="A38" s="45" t="s">
         <v>17</v>
       </c>
       <c r="B38" s="18">
         <v>1.2</v>
       </c>
-      <c r="C38" s="43">
+      <c r="C38" s="48">
         <v>1</v>
       </c>
-      <c r="D38" s="27" t="s">
+      <c r="D38" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E38" s="40" t="s">
+      <c r="E38" s="45" t="s">
         <v>13</v>
       </c>
       <c r="F38" s="18">
         <v>1.5</v>
       </c>
-      <c r="G38" s="27" t="s">
+      <c r="G38" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="H38" s="40" t="s">
+      <c r="H38" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="I38" s="43">
+      <c r="I38" s="48">
         <v>1</v>
       </c>
-      <c r="J38" s="27" t="s">
+      <c r="J38" s="30" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A39" s="41"/>
+      <c r="A39" s="46"/>
       <c r="B39" s="2">
         <v>1.5</v>
       </c>
-      <c r="C39" s="32"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="41"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="46"/>
       <c r="F39" s="2">
         <v>2</v>
       </c>
-      <c r="G39" s="25"/>
-      <c r="H39" s="41"/>
-      <c r="I39" s="32"/>
-      <c r="J39" s="25"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="46"/>
+      <c r="I39" s="49"/>
+      <c r="J39" s="31"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A40" s="41"/>
+      <c r="A40" s="46"/>
       <c r="B40" s="2">
         <v>1.7</v>
       </c>
-      <c r="C40" s="32"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="41"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="46"/>
       <c r="F40" s="2">
         <v>2.5</v>
       </c>
-      <c r="G40" s="25"/>
-      <c r="H40" s="41"/>
-      <c r="I40" s="32">
+      <c r="G40" s="31"/>
+      <c r="H40" s="46"/>
+      <c r="I40" s="49">
         <v>2</v>
       </c>
-      <c r="J40" s="25"/>
+      <c r="J40" s="31"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A41" s="41"/>
+      <c r="A41" s="46"/>
       <c r="B41" s="2">
         <v>2</v>
       </c>
-      <c r="C41" s="32"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="41"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="46"/>
       <c r="F41" s="2">
         <v>3</v>
       </c>
-      <c r="G41" s="25"/>
-      <c r="H41" s="41"/>
-      <c r="I41" s="32"/>
-      <c r="J41" s="25"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="46"/>
+      <c r="I41" s="49"/>
+      <c r="J41" s="31"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A42" s="41"/>
+      <c r="A42" s="46"/>
       <c r="B42" s="2">
         <v>2.5</v>
       </c>
-      <c r="C42" s="32"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="36" t="s">
+      <c r="C42" s="49"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="50" t="s">
         <v>14</v>
       </c>
       <c r="F42" s="2">
         <v>1.5</v>
       </c>
-      <c r="G42" s="25"/>
-      <c r="H42" s="36" t="s">
+      <c r="G42" s="31"/>
+      <c r="H42" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="I42" s="32">
+      <c r="I42" s="49">
         <v>1</v>
       </c>
-      <c r="J42" s="25"/>
+      <c r="J42" s="31"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A43" s="41"/>
+      <c r="A43" s="46"/>
       <c r="B43" s="2">
         <v>3</v>
       </c>
-      <c r="C43" s="32"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="36"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="50"/>
       <c r="F43" s="2">
         <v>2</v>
       </c>
-      <c r="G43" s="25"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="32"/>
-      <c r="J43" s="25"/>
+      <c r="G43" s="31"/>
+      <c r="H43" s="50"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="31"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A44" s="41"/>
+      <c r="A44" s="46"/>
       <c r="B44" s="2">
         <v>1.2</v>
       </c>
-      <c r="C44" s="32">
+      <c r="C44" s="49">
         <v>2</v>
       </c>
-      <c r="D44" s="25"/>
-      <c r="E44" s="36"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="50"/>
       <c r="F44" s="2">
         <v>2.5</v>
       </c>
-      <c r="G44" s="25"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="32">
+      <c r="G44" s="31"/>
+      <c r="H44" s="50"/>
+      <c r="I44" s="49">
         <v>2</v>
       </c>
-      <c r="J44" s="25"/>
+      <c r="J44" s="31"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A45" s="41"/>
+      <c r="A45" s="46"/>
       <c r="B45" s="2">
         <v>1.5</v>
       </c>
-      <c r="C45" s="32"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="36"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="50"/>
       <c r="F45" s="2">
         <v>3</v>
       </c>
-      <c r="G45" s="25"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="32"/>
-      <c r="J45" s="25"/>
+      <c r="G45" s="31"/>
+      <c r="H45" s="50"/>
+      <c r="I45" s="49"/>
+      <c r="J45" s="31"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A46" s="41"/>
+      <c r="A46" s="46"/>
       <c r="B46" s="2">
         <v>1.7</v>
       </c>
-      <c r="C46" s="32"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="36" t="s">
+      <c r="C46" s="49"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="50" t="s">
         <v>15</v>
       </c>
       <c r="F46" s="2">
         <v>1.5</v>
       </c>
-      <c r="G46" s="25"/>
-      <c r="H46" s="36" t="s">
+      <c r="G46" s="31"/>
+      <c r="H46" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="I46" s="32">
+      <c r="I46" s="49">
         <v>1</v>
       </c>
-      <c r="J46" s="25"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A47" s="41"/>
+      <c r="A47" s="46"/>
       <c r="B47" s="2">
         <v>2</v>
       </c>
-      <c r="C47" s="32"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="36"/>
+      <c r="C47" s="49"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="50"/>
       <c r="F47" s="2">
         <v>2</v>
       </c>
-      <c r="G47" s="25"/>
-      <c r="H47" s="36"/>
-      <c r="I47" s="32"/>
-      <c r="J47" s="25"/>
+      <c r="G47" s="31"/>
+      <c r="H47" s="50"/>
+      <c r="I47" s="49"/>
+      <c r="J47" s="31"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A48" s="41"/>
+      <c r="A48" s="46"/>
       <c r="B48" s="2">
         <v>2.5</v>
       </c>
-      <c r="C48" s="32"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="36"/>
+      <c r="C48" s="49"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="50"/>
       <c r="F48" s="2">
         <v>2.5</v>
       </c>
-      <c r="G48" s="25"/>
-      <c r="H48" s="36"/>
-      <c r="I48" s="32">
+      <c r="G48" s="31"/>
+      <c r="H48" s="50"/>
+      <c r="I48" s="49">
         <v>2</v>
       </c>
-      <c r="J48" s="25"/>
+      <c r="J48" s="31"/>
     </row>
     <row r="49" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="42"/>
+      <c r="A49" s="47"/>
       <c r="B49" s="20">
         <v>3</v>
       </c>
-      <c r="C49" s="33"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="37"/>
+      <c r="C49" s="51"/>
+      <c r="D49" s="34"/>
+      <c r="E49" s="52"/>
       <c r="F49" s="20">
         <v>3</v>
       </c>
-      <c r="G49" s="28"/>
-      <c r="H49" s="37"/>
-      <c r="I49" s="33"/>
-      <c r="J49" s="28"/>
+      <c r="G49" s="34"/>
+      <c r="H49" s="52"/>
+      <c r="I49" s="51"/>
+      <c r="J49" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="J14:J25"/>
-    <mergeCell ref="J26:J35"/>
-    <mergeCell ref="G26:G30"/>
-    <mergeCell ref="G32:G37"/>
-    <mergeCell ref="J38:J49"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="G2:G13"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="C8:C13"/>
-    <mergeCell ref="C2:C7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="H6:H9"/>
-    <mergeCell ref="H10:H13"/>
-    <mergeCell ref="J2:J13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="C14:C19"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="H18:H21"/>
-    <mergeCell ref="G14:G25"/>
-    <mergeCell ref="C26:C31"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="C20:C25"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="H22:H25"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="C44:C49"/>
-    <mergeCell ref="I44:I45"/>
-    <mergeCell ref="E46:E49"/>
-    <mergeCell ref="H46:H49"/>
-    <mergeCell ref="I46:I47"/>
-    <mergeCell ref="I36:I37"/>
-    <mergeCell ref="J36:J37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="C38:C43"/>
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="H38:H41"/>
-    <mergeCell ref="I38:I39"/>
-    <mergeCell ref="I40:I41"/>
-    <mergeCell ref="C32:C37"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="E34:E37"/>
-    <mergeCell ref="H34:H37"/>
-    <mergeCell ref="I34:I35"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="I48:I49"/>
     <mergeCell ref="D2:D13"/>
@@ -9816,6 +9751,71 @@
     <mergeCell ref="I30:I31"/>
     <mergeCell ref="G38:G49"/>
     <mergeCell ref="D38:D49"/>
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="C38:C43"/>
+    <mergeCell ref="E38:E41"/>
+    <mergeCell ref="H38:H41"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="I40:I41"/>
+    <mergeCell ref="C44:C49"/>
+    <mergeCell ref="I44:I45"/>
+    <mergeCell ref="E46:E49"/>
+    <mergeCell ref="H46:H49"/>
+    <mergeCell ref="I46:I47"/>
+    <mergeCell ref="C26:C31"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="C32:C37"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="E34:E37"/>
+    <mergeCell ref="H34:H37"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="J2:J13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="C14:C19"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="H18:H21"/>
+    <mergeCell ref="G14:G25"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="C20:C25"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="H22:H25"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="C8:C13"/>
+    <mergeCell ref="C2:C7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="G2:G13"/>
+    <mergeCell ref="J14:J25"/>
+    <mergeCell ref="J26:J35"/>
+    <mergeCell ref="G26:G30"/>
+    <mergeCell ref="G32:G37"/>
+    <mergeCell ref="J38:J49"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="I36:I37"/>
+    <mergeCell ref="J36:J37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added code to measure time processing
</commit_message>
<xml_diff>
--- a/detect_methods_comp.xlsx
+++ b/detect_methods_comp.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iwaya\Escritorio\Code\FaceRecogServer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A78C89-2BA5-4D0D-8586-8DFE5E7B24CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABADF2DA-842B-4ECF-AE0B-E4DB6A229E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Resize (OpenCV)" sheetId="2" r:id="rId1"/>
-    <sheet name="get_frontal_face_detector()" sheetId="1" r:id="rId2"/>
-    <sheet name="DeepNeuralNetworks Methods" sheetId="3" r:id="rId3"/>
-    <sheet name="Combinación métodos" sheetId="4" r:id="rId4"/>
-    <sheet name="Tiempos procesamiento" sheetId="5" r:id="rId5"/>
+    <sheet name="Resultados" sheetId="6" r:id="rId1"/>
+    <sheet name="Resize (OpenCV)" sheetId="2" r:id="rId2"/>
+    <sheet name="get_frontal_face_detector()" sheetId="1" r:id="rId3"/>
+    <sheet name="DeepNeuralNetworks Methods" sheetId="3" r:id="rId4"/>
+    <sheet name="Combinación métodos" sheetId="4" r:id="rId5"/>
+    <sheet name="Tiempos procesamiento" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="69">
   <si>
     <t>Up Sampling [dlib.get_frontal_face_detector()]</t>
   </si>
@@ -182,6 +183,72 @@
   <si>
     <t>4, 2</t>
   </si>
+  <si>
+    <t>Reconocimiento facial</t>
+  </si>
+  <si>
+    <t>Si*</t>
+  </si>
+  <si>
+    <t>0.38 segundos</t>
+  </si>
+  <si>
+    <t>11 segundos</t>
+  </si>
+  <si>
+    <t>1.5 segundos</t>
+  </si>
+  <si>
+    <t>Número de rostros en escena</t>
+  </si>
+  <si>
+    <t>Resolución imágenes Go1</t>
+  </si>
+  <si>
+    <t>1856x800</t>
+  </si>
+  <si>
+    <t>Promedio detección facial y envió del face chip</t>
+  </si>
+  <si>
+    <t>Promedio de extracción de características y reconocimiento facial</t>
+  </si>
+  <si>
+    <t>Promedio envió imagezmq</t>
+  </si>
+  <si>
+    <t>1 metro</t>
+  </si>
+  <si>
+    <t>2 metros</t>
+  </si>
+  <si>
+    <t>3 metros</t>
+  </si>
+  <si>
+    <t>4 metros</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>928x400</t>
+  </si>
+  <si>
+    <t>*Si la calidad de la imagen transmitida internamente lo permite, en general la calidad de la imagen era muy baja como para hacer FR</t>
+  </si>
+  <si>
+    <t>11.5 segundos</t>
+  </si>
+  <si>
+    <t>1 segundo</t>
+  </si>
+  <si>
+    <t>0.4 segundos</t>
+  </si>
+  <si>
+    <t>928x400 (re-escalado por 2 en placa receptora interna)</t>
+  </si>
 </sst>
 </file>
 
@@ -204,7 +271,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,8 +326,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -514,26 +587,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -618,6 +671,15 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -625,9 +687,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -727,12 +786,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -7847,29 +7900,306 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD554FA1-10E3-4A88-8A1D-54AF58A25FC5}">
+  <dimension ref="A1:G25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="28">
+        <v>1</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="28"/>
+      <c r="B6" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="A2:A13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6706964-F93E-4934-BEB2-8D6878ECF54C}">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView zoomScale="103" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="12" width="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>27</v>
       </c>
@@ -7897,7 +8227,7 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
@@ -7941,7 +8271,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -7989,7 +8319,7 @@
         <v>1.1792592592592592</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -8037,7 +8367,7 @@
         <v>3.2364197530864196</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -8085,7 +8415,7 @@
         <v>6.2976543209876548</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -8133,7 +8463,7 @@
         <v>10.856419753086421</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -8181,7 +8511,7 @@
         <v>16.636172839506173</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -8228,405 +8558,6 @@
         <f t="shared" si="1"/>
         <v>23.849876543209877</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q13"/>
-  <sheetViews>
-    <sheetView zoomScale="84" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="44.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="9.1796875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="5">
-        <v>37.4</v>
-      </c>
-      <c r="E3" s="5">
-        <f>D3/60</f>
-        <v>0.62333333333333329</v>
-      </c>
-      <c r="F3" s="8">
-        <f>D3/37</f>
-        <v>1.0108108108108107</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M3" s="5">
-        <v>98.11</v>
-      </c>
-      <c r="N3" s="5">
-        <f t="shared" ref="N3:N8" si="0">M3/60</f>
-        <v>1.6351666666666667</v>
-      </c>
-      <c r="O3" s="8">
-        <f>M3/81</f>
-        <v>1.2112345679012346</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="5">
-        <v>76.239999999999995</v>
-      </c>
-      <c r="E4" s="5">
-        <f t="shared" ref="E4:E8" si="1">D4/60</f>
-        <v>1.2706666666666666</v>
-      </c>
-      <c r="F4" s="8">
-        <f t="shared" ref="F4:F8" si="2">D4/37</f>
-        <v>2.0605405405405404</v>
-      </c>
-      <c r="H4" s="2">
-        <v>1</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M4" s="5">
-        <v>268.89999999999998</v>
-      </c>
-      <c r="N4" s="5">
-        <f t="shared" si="0"/>
-        <v>4.4816666666666665</v>
-      </c>
-      <c r="O4" s="8">
-        <f t="shared" ref="O4:O6" si="3">M4/81</f>
-        <v>3.3197530864197526</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" s="6">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="5">
-        <v>191.54</v>
-      </c>
-      <c r="E5" s="5">
-        <f t="shared" si="1"/>
-        <v>3.192333333333333</v>
-      </c>
-      <c r="F5" s="8">
-        <f t="shared" si="2"/>
-        <v>5.1767567567567569</v>
-      </c>
-      <c r="H5" s="2">
-        <v>2</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M5" s="5">
-        <v>956.49</v>
-      </c>
-      <c r="N5" s="5">
-        <f t="shared" si="0"/>
-        <v>15.9415</v>
-      </c>
-      <c r="O5" s="8">
-        <f t="shared" si="3"/>
-        <v>11.808518518518518</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="5">
-        <v>419.84</v>
-      </c>
-      <c r="E6" s="5">
-        <f t="shared" si="1"/>
-        <v>6.9973333333333327</v>
-      </c>
-      <c r="F6" s="8">
-        <f t="shared" si="2"/>
-        <v>11.347027027027027</v>
-      </c>
-      <c r="H6" s="2">
-        <v>3</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M6" s="5">
-        <v>3674.01</v>
-      </c>
-      <c r="N6" s="5">
-        <f t="shared" si="0"/>
-        <v>61.233500000000006</v>
-      </c>
-      <c r="O6" s="8">
-        <f t="shared" si="3"/>
-        <v>45.358148148148153</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A7" s="7">
-        <v>4</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="5">
-        <v>1559.89</v>
-      </c>
-      <c r="E7" s="5">
-        <f t="shared" si="1"/>
-        <v>25.99816666666667</v>
-      </c>
-      <c r="F7" s="8">
-        <f t="shared" si="2"/>
-        <v>42.159189189189192</v>
-      </c>
-      <c r="H7" s="2">
-        <v>4</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M7" s="5">
-        <v>14483.55</v>
-      </c>
-      <c r="N7" s="5">
-        <f t="shared" si="0"/>
-        <v>241.39249999999998</v>
-      </c>
-      <c r="O7" s="8">
-        <f>M7/81</f>
-        <v>178.80925925925925</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" s="6">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="5">
-        <v>5878.92</v>
-      </c>
-      <c r="E8" s="5">
-        <f t="shared" si="1"/>
-        <v>97.981999999999999</v>
-      </c>
-      <c r="F8" s="8">
-        <f t="shared" si="2"/>
-        <v>158.88972972972974</v>
-      </c>
-      <c r="H8" s="2">
-        <v>5</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M8" s="5">
-        <v>59016.9</v>
-      </c>
-      <c r="N8" s="5">
-        <f t="shared" si="0"/>
-        <v>983.61500000000001</v>
-      </c>
-      <c r="O8" s="8">
-        <f>M8/81</f>
-        <v>728.60370370370367</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8636,30 +8567,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EDFC79-1BF5-4D0E-ADD4-A69D2D4846CD}">
-  <dimension ref="A1:O5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView zoomScale="92" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView zoomScale="84" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" customWidth="1"/>
-    <col min="7" max="7" width="11.54296875" customWidth="1"/>
-    <col min="8" max="8" width="42.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="4.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>27</v>
       </c>
@@ -8672,24 +8604,16 @@
       <c r="D1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
       <c r="H1" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>5</v>
@@ -8703,12 +8627,11 @@
       <c r="E2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="11"/>
       <c r="H2" s="13" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="I2" s="13" t="s">
         <v>17</v>
@@ -8728,34 +8651,33 @@
       <c r="N2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="21" t="s">
+      <c r="O2" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
-        <v>13</v>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" s="5">
-        <v>152.66999999999999</v>
+        <v>37.4</v>
       </c>
       <c r="E3" s="5">
         <f>D3/60</f>
-        <v>2.5444999999999998</v>
+        <v>0.62333333333333329</v>
       </c>
       <c r="F3" s="8">
         <f>D3/37</f>
-        <v>4.1262162162162159</v>
-      </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="6" t="s">
-        <v>13</v>
+        <v>1.0108108108108107</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>1</v>
@@ -8764,47 +8686,46 @@
         <v>1</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M3" s="2">
-        <v>1305.19</v>
+        <v>1</v>
+      </c>
+      <c r="M3" s="5">
+        <v>98.11</v>
       </c>
       <c r="N3" s="5">
-        <f>M3/60</f>
-        <v>21.753166666666669</v>
+        <f t="shared" ref="N3:N8" si="0">M3/60</f>
+        <v>1.6351666666666667</v>
       </c>
       <c r="O3" s="8">
         <f>M3/81</f>
-        <v>16.113456790123458</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="4" t="s">
+        <v>1.2112345679012346</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
         <v>1</v>
       </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="D4" s="5">
-        <v>152.69</v>
+        <v>76.239999999999995</v>
       </c>
       <c r="E4" s="5">
-        <f t="shared" ref="E4:E5" si="0">D4/60</f>
-        <v>2.5448333333333335</v>
+        <f t="shared" ref="E4:E8" si="1">D4/60</f>
+        <v>1.2706666666666666</v>
       </c>
       <c r="F4" s="8">
-        <f t="shared" ref="F4:F5" si="1">D4/37</f>
-        <v>4.1267567567567571</v>
-      </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="6" t="s">
-        <v>14</v>
+        <f t="shared" ref="F4:F8" si="2">D4/37</f>
+        <v>2.0605405405405404</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>1</v>
@@ -8813,26 +8734,26 @@
         <v>1</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M4" s="2">
-        <v>1674.66</v>
+        <v>1</v>
+      </c>
+      <c r="M4" s="5">
+        <v>268.89999999999998</v>
       </c>
       <c r="N4" s="5">
-        <f>M4/60</f>
-        <v>27.911000000000001</v>
+        <f t="shared" si="0"/>
+        <v>4.4816666666666665</v>
       </c>
       <c r="O4" s="8">
-        <f t="shared" ref="O4:O5" si="2">M4/81</f>
-        <v>20.674814814814816</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
-        <v>15</v>
+        <f t="shared" ref="O4:O6" si="3">M4/81</f>
+        <v>3.3197530864197526</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -8841,25 +8762,24 @@
         <v>1</v>
       </c>
       <c r="D5" s="5">
-        <v>1212.56</v>
+        <v>191.54</v>
       </c>
       <c r="E5" s="5">
-        <f t="shared" si="0"/>
-        <v>20.209333333333333</v>
+        <f t="shared" si="1"/>
+        <v>3.192333333333333</v>
       </c>
       <c r="F5" s="8">
-        <f t="shared" si="1"/>
-        <v>32.77189189189189</v>
-      </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="6" t="s">
-        <v>15</v>
+        <f t="shared" si="2"/>
+        <v>5.1767567567567569</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>4</v>
@@ -8868,16 +8788,175 @@
         <v>4</v>
       </c>
       <c r="M5" s="5">
-        <v>12024.66</v>
+        <v>956.49</v>
       </c>
       <c r="N5" s="5">
-        <f>M5/60</f>
-        <v>200.411</v>
+        <f t="shared" si="0"/>
+        <v>15.9415</v>
       </c>
       <c r="O5" s="8">
+        <f t="shared" si="3"/>
+        <v>11.808518518518518</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="5">
+        <v>419.84</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" si="1"/>
+        <v>6.9973333333333327</v>
+      </c>
+      <c r="F6" s="8">
         <f t="shared" si="2"/>
-        <v>148.45259259259259</v>
-      </c>
+        <v>11.347027027027027</v>
+      </c>
+      <c r="H6" s="2">
+        <v>3</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="5">
+        <v>3674.01</v>
+      </c>
+      <c r="N6" s="5">
+        <f t="shared" si="0"/>
+        <v>61.233500000000006</v>
+      </c>
+      <c r="O6" s="8">
+        <f t="shared" si="3"/>
+        <v>45.358148148148153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1559.89</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="1"/>
+        <v>25.99816666666667</v>
+      </c>
+      <c r="F7" s="8">
+        <f t="shared" si="2"/>
+        <v>42.159189189189192</v>
+      </c>
+      <c r="H7" s="2">
+        <v>4</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M7" s="5">
+        <v>14483.55</v>
+      </c>
+      <c r="N7" s="5">
+        <f t="shared" si="0"/>
+        <v>241.39249999999998</v>
+      </c>
+      <c r="O7" s="8">
+        <f>M7/81</f>
+        <v>178.80925925925925</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="5">
+        <v>5878.92</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="1"/>
+        <v>97.981999999999999</v>
+      </c>
+      <c r="F8" s="8">
+        <f t="shared" si="2"/>
+        <v>158.88972972972974</v>
+      </c>
+      <c r="H8" s="2">
+        <v>5</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M8" s="5">
+        <v>59016.9</v>
+      </c>
+      <c r="N8" s="5">
+        <f t="shared" si="0"/>
+        <v>983.61500000000001</v>
+      </c>
+      <c r="O8" s="8">
+        <f>M8/81</f>
+        <v>728.60370370370367</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8887,976 +8966,1227 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EDFC79-1BF5-4D0E-ADD4-A69D2D4846CD}">
+  <dimension ref="A1:O5"/>
+  <sheetViews>
+    <sheetView zoomScale="92" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="11"/>
+      <c r="H2" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
+        <v>152.66999999999999</v>
+      </c>
+      <c r="E3" s="5">
+        <f>D3/60</f>
+        <v>2.5444999999999998</v>
+      </c>
+      <c r="F3" s="8">
+        <f>D3/37</f>
+        <v>4.1262162162162159</v>
+      </c>
+      <c r="G3" s="12"/>
+      <c r="H3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="2">
+        <v>1305.19</v>
+      </c>
+      <c r="N3" s="5">
+        <f>M3/60</f>
+        <v>21.753166666666669</v>
+      </c>
+      <c r="O3" s="8">
+        <f>M3/81</f>
+        <v>16.113456790123458</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
+        <v>152.69</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" ref="E4:E5" si="0">D4/60</f>
+        <v>2.5448333333333335</v>
+      </c>
+      <c r="F4" s="8">
+        <f t="shared" ref="F4:F5" si="1">D4/37</f>
+        <v>4.1267567567567571</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" s="2">
+        <v>1674.66</v>
+      </c>
+      <c r="N4" s="5">
+        <f>M4/60</f>
+        <v>27.911000000000001</v>
+      </c>
+      <c r="O4" s="8">
+        <f t="shared" ref="O4:O5" si="2">M4/81</f>
+        <v>20.674814814814816</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1212.56</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" si="0"/>
+        <v>20.209333333333333</v>
+      </c>
+      <c r="F5" s="8">
+        <f t="shared" si="1"/>
+        <v>32.77189189189189</v>
+      </c>
+      <c r="G5" s="12"/>
+      <c r="H5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" s="5">
+        <v>12024.66</v>
+      </c>
+      <c r="N5" s="5">
+        <f>M5/60</f>
+        <v>200.411</v>
+      </c>
+      <c r="O5" s="8">
+        <f t="shared" si="2"/>
+        <v>148.45259259259259</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB5E59B-51C7-438E-AB32-5EE19B87C996}">
   <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView zoomScale="102" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26:I27"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7265625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7265625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.81640625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="8.54296875" style="14" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="14" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="14" customWidth="1"/>
     <col min="8" max="8" width="15" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.6328125" style="14" customWidth="1"/>
-    <col min="10" max="10" width="9.1796875" style="14" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" style="14" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="56"/>
+      <c r="C1" s="58"/>
       <c r="D1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="56"/>
+      <c r="F1" s="58"/>
       <c r="G1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="H1" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="56"/>
+      <c r="I1" s="58"/>
       <c r="J1" s="25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="27" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="16">
         <v>1.2</v>
       </c>
-      <c r="C2" s="49">
+      <c r="C2" s="51">
         <v>1</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="30" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="16">
         <v>1.5</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="49">
+      <c r="I2" s="51">
         <v>1</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="34" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="28"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="31"/>
       <c r="B3" s="15">
         <v>1.5</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="28"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="31"/>
       <c r="F3" s="15">
         <v>2</v>
       </c>
-      <c r="G3" s="33"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="33"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="28"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="35"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="31"/>
       <c r="B4" s="15">
         <v>1.7</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="28"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="31"/>
       <c r="F4" s="15">
         <v>2.5</v>
       </c>
-      <c r="G4" s="33"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="43">
+      <c r="G4" s="35"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="45">
         <v>2</v>
       </c>
-      <c r="J4" s="33"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="28"/>
+      <c r="J4" s="35"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="31"/>
       <c r="B5" s="15">
         <v>2</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="28"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="31"/>
       <c r="F5" s="15">
         <v>3</v>
       </c>
-      <c r="G5" s="33"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="33"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="28"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="35"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="31"/>
       <c r="B6" s="15">
         <v>2.5</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="42" t="s">
+      <c r="C6" s="45"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="44" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="15">
         <v>1.5</v>
       </c>
-      <c r="G6" s="33"/>
-      <c r="H6" s="42" t="s">
+      <c r="G6" s="35"/>
+      <c r="H6" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="43">
+      <c r="I6" s="45">
         <v>1</v>
       </c>
-      <c r="J6" s="33"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="28"/>
+      <c r="J6" s="35"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="31"/>
       <c r="B7" s="15">
         <v>3</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="42"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="44"/>
       <c r="F7" s="15">
         <v>2</v>
       </c>
-      <c r="G7" s="33"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="33"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="28"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="35"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="31"/>
       <c r="B8" s="15">
         <v>1.2</v>
       </c>
-      <c r="C8" s="43">
+      <c r="C8" s="45">
         <v>2</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="42"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="44"/>
       <c r="F8" s="15">
         <v>2.5</v>
       </c>
-      <c r="G8" s="33"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="43">
+      <c r="G8" s="35"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="45">
         <v>2</v>
       </c>
-      <c r="J8" s="33"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="28"/>
+      <c r="J8" s="35"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="31"/>
       <c r="B9" s="15">
         <v>1.5</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="42"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="44"/>
       <c r="F9" s="15">
         <v>3</v>
       </c>
-      <c r="G9" s="33"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="33"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="28"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="35"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="31"/>
       <c r="B10" s="15">
         <v>1.7</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="42" t="s">
+      <c r="C10" s="45"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="44" t="s">
         <v>15</v>
       </c>
       <c r="F10" s="15">
         <v>1.5</v>
       </c>
-      <c r="G10" s="33"/>
-      <c r="H10" s="42" t="s">
+      <c r="G10" s="35"/>
+      <c r="H10" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="43">
+      <c r="I10" s="45">
         <v>1</v>
       </c>
-      <c r="J10" s="33"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="28"/>
+      <c r="J10" s="35"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="31"/>
       <c r="B11" s="15">
         <v>2</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="42"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="44"/>
       <c r="F11" s="15">
         <v>2</v>
       </c>
-      <c r="G11" s="33"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="33"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="28"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="35"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="31"/>
       <c r="B12" s="15">
         <v>2.5</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="42"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="44"/>
       <c r="F12" s="15">
         <v>2.5</v>
       </c>
-      <c r="G12" s="33"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="43">
+      <c r="G12" s="35"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="45">
         <v>2</v>
       </c>
-      <c r="J12" s="33"/>
-    </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="29"/>
+      <c r="J12" s="35"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="32"/>
       <c r="B13" s="17">
         <v>3</v>
       </c>
-      <c r="C13" s="54"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="55"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="57"/>
       <c r="F13" s="17">
         <v>3</v>
       </c>
-      <c r="G13" s="34"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="34"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="44" t="s">
+      <c r="G13" s="36"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="36"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="46" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="18">
         <v>1.2</v>
       </c>
-      <c r="C14" s="47">
+      <c r="C14" s="49">
         <v>1</v>
       </c>
-      <c r="D14" s="35" t="s">
+      <c r="D14" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="44" t="s">
+      <c r="E14" s="46" t="s">
         <v>13</v>
       </c>
       <c r="F14" s="18">
         <v>1.5</v>
       </c>
-      <c r="G14" s="32" t="s">
+      <c r="G14" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="H14" s="44" t="s">
+      <c r="H14" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="47">
+      <c r="I14" s="49">
         <v>1</v>
       </c>
-      <c r="J14" s="32" t="s">
+      <c r="J14" s="34" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="45"/>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="47"/>
       <c r="B15" s="2">
         <v>1.5</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="45"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="47"/>
       <c r="F15" s="2">
         <v>2</v>
       </c>
-      <c r="G15" s="33"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="33"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="45"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="35"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="47"/>
       <c r="B16" s="2">
         <v>1.7</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="45"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="47"/>
       <c r="F16" s="2">
         <v>2.5</v>
       </c>
-      <c r="G16" s="33"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="30">
+      <c r="G16" s="35"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="28">
         <v>2</v>
       </c>
-      <c r="J16" s="33"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="45"/>
+      <c r="J16" s="35"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="47"/>
       <c r="B17" s="2">
         <v>2</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="45"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="47"/>
       <c r="F17" s="2">
         <v>3</v>
       </c>
-      <c r="G17" s="33"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="33"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="45"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="35"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="47"/>
       <c r="B18" s="2">
         <v>2.5</v>
       </c>
-      <c r="C18" s="30"/>
-      <c r="D18" s="38" t="s">
+      <c r="C18" s="28"/>
+      <c r="D18" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="41" t="s">
+      <c r="E18" s="43" t="s">
         <v>14</v>
       </c>
       <c r="F18" s="2">
         <v>1.5</v>
       </c>
-      <c r="G18" s="33"/>
-      <c r="H18" s="41" t="s">
+      <c r="G18" s="35"/>
+      <c r="H18" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="I18" s="30">
+      <c r="I18" s="28">
         <v>1</v>
       </c>
-      <c r="J18" s="33"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="45"/>
+      <c r="J18" s="35"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="47"/>
       <c r="B19" s="2">
         <v>3</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="41"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="43"/>
       <c r="F19" s="2">
         <v>2</v>
       </c>
-      <c r="G19" s="33"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="33"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="45"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="35"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="47"/>
       <c r="B20" s="2">
         <v>1.2</v>
       </c>
-      <c r="C20" s="30">
+      <c r="C20" s="28">
         <v>2</v>
       </c>
       <c r="D20" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="41"/>
+      <c r="E20" s="43"/>
       <c r="F20" s="2">
         <v>2.5</v>
       </c>
-      <c r="G20" s="33"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="30">
+      <c r="G20" s="35"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="28">
         <v>2</v>
       </c>
-      <c r="J20" s="33"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" s="45"/>
+      <c r="J20" s="35"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="47"/>
       <c r="B21" s="2">
         <v>1.5</v>
       </c>
-      <c r="C21" s="30"/>
-      <c r="D21" s="38" t="s">
+      <c r="C21" s="28"/>
+      <c r="D21" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="41"/>
+      <c r="E21" s="43"/>
       <c r="F21" s="2">
         <v>3</v>
       </c>
-      <c r="G21" s="33"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="33"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="45"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="35"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="47"/>
       <c r="B22" s="2">
         <v>1.7</v>
       </c>
-      <c r="C22" s="30"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="41" t="s">
+      <c r="C22" s="28"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="43" t="s">
         <v>15</v>
       </c>
       <c r="F22" s="2">
         <v>1.5</v>
       </c>
-      <c r="G22" s="33"/>
-      <c r="H22" s="41" t="s">
+      <c r="G22" s="35"/>
+      <c r="H22" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="I22" s="30">
+      <c r="I22" s="28">
         <v>1</v>
       </c>
-      <c r="J22" s="33"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="45"/>
+      <c r="J22" s="35"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="47"/>
       <c r="B23" s="2">
         <v>2</v>
       </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="41"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="43"/>
       <c r="F23" s="2">
         <v>2</v>
       </c>
-      <c r="G23" s="33"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="33"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" s="45"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="35"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="47"/>
       <c r="B24" s="2">
         <v>2.5</v>
       </c>
-      <c r="C24" s="30"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="41"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="43"/>
       <c r="F24" s="2">
         <v>2.5</v>
       </c>
-      <c r="G24" s="33"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="30">
+      <c r="G24" s="35"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="28">
         <v>2</v>
       </c>
-      <c r="J24" s="33"/>
-    </row>
-    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="46"/>
+      <c r="J24" s="35"/>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="48"/>
       <c r="B25" s="20">
         <v>3</v>
       </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="48"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="50"/>
       <c r="F25" s="20">
         <v>3</v>
       </c>
-      <c r="G25" s="34"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="34"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A26" s="27" t="s">
+      <c r="G25" s="36"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="36"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="30" t="s">
         <v>18</v>
       </c>
       <c r="B26" s="16">
         <v>1.2</v>
       </c>
-      <c r="C26" s="49">
+      <c r="C26" s="51">
         <v>1</v>
       </c>
-      <c r="D26" s="35" t="s">
+      <c r="D26" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="27" t="s">
+      <c r="E26" s="30" t="s">
         <v>13</v>
       </c>
       <c r="F26" s="16">
         <v>1.5</v>
       </c>
-      <c r="G26" s="35" t="s">
+      <c r="G26" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="H26" s="50" t="s">
+      <c r="H26" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="I26" s="52">
+      <c r="I26" s="54">
         <v>1</v>
       </c>
-      <c r="J26" s="32" t="s">
+      <c r="J26" s="34" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A27" s="28"/>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="31"/>
       <c r="B27" s="15">
         <v>1.5</v>
       </c>
-      <c r="C27" s="43"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="28"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="31"/>
       <c r="F27" s="15">
         <v>2</v>
       </c>
-      <c r="G27" s="36"/>
-      <c r="H27" s="51"/>
-      <c r="I27" s="53"/>
-      <c r="J27" s="33"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A28" s="28"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="55"/>
+      <c r="J27" s="35"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="31"/>
       <c r="B28" s="15">
         <v>1.7</v>
       </c>
-      <c r="C28" s="43"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="28"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="31"/>
       <c r="F28" s="15">
         <v>2.5</v>
       </c>
-      <c r="G28" s="36"/>
-      <c r="H28" s="51"/>
-      <c r="I28" s="53">
+      <c r="G28" s="38"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="55">
         <v>2</v>
       </c>
-      <c r="J28" s="33"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A29" s="28"/>
+      <c r="J28" s="35"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="31"/>
       <c r="B29" s="15">
         <v>2</v>
       </c>
-      <c r="C29" s="43"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="28"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="31"/>
       <c r="F29" s="15">
         <v>3</v>
       </c>
-      <c r="G29" s="36"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="53"/>
-      <c r="J29" s="33"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A30" s="28"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="35"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="31"/>
       <c r="B30" s="15">
         <v>2.5</v>
       </c>
-      <c r="C30" s="43"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="42" t="s">
+      <c r="C30" s="45"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="44" t="s">
         <v>14</v>
       </c>
       <c r="F30" s="15">
         <v>1.5</v>
       </c>
-      <c r="G30" s="37"/>
-      <c r="H30" s="42" t="s">
+      <c r="G30" s="39"/>
+      <c r="H30" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="I30" s="43">
+      <c r="I30" s="45">
         <v>1</v>
       </c>
-      <c r="J30" s="33"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A31" s="28"/>
+      <c r="J30" s="35"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="31"/>
       <c r="B31" s="15">
         <v>3</v>
       </c>
-      <c r="C31" s="43"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="42"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="44"/>
       <c r="F31" s="15">
         <v>2</v>
       </c>
       <c r="G31" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="H31" s="42"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="33"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A32" s="28"/>
+      <c r="H31" s="44"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="35"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="31"/>
       <c r="B32" s="15">
         <v>1.2</v>
       </c>
-      <c r="C32" s="43">
+      <c r="C32" s="45">
         <v>2</v>
       </c>
-      <c r="D32" s="36"/>
-      <c r="E32" s="42"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="44"/>
       <c r="F32" s="15">
         <v>2.5</v>
       </c>
-      <c r="G32" s="58" t="s">
+      <c r="G32" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="H32" s="42"/>
-      <c r="I32" s="43">
+      <c r="H32" s="44"/>
+      <c r="I32" s="45">
         <v>2</v>
       </c>
-      <c r="J32" s="33"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A33" s="28"/>
+      <c r="J32" s="35"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="31"/>
       <c r="B33" s="15">
         <v>1.5</v>
       </c>
-      <c r="C33" s="43"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="42"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="44"/>
       <c r="F33" s="15">
         <v>3</v>
       </c>
-      <c r="G33" s="36"/>
-      <c r="H33" s="42"/>
-      <c r="I33" s="43"/>
-      <c r="J33" s="33"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A34" s="28"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="35"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="31"/>
       <c r="B34" s="15">
         <v>1.7</v>
       </c>
-      <c r="C34" s="43"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="42" t="s">
+      <c r="C34" s="45"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="44" t="s">
         <v>15</v>
       </c>
       <c r="F34" s="15">
         <v>1.5</v>
       </c>
-      <c r="G34" s="36"/>
-      <c r="H34" s="42" t="s">
+      <c r="G34" s="38"/>
+      <c r="H34" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="I34" s="43">
+      <c r="I34" s="45">
         <v>1</v>
       </c>
-      <c r="J34" s="33"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A35" s="28"/>
+      <c r="J34" s="35"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="31"/>
       <c r="B35" s="15">
         <v>2</v>
       </c>
-      <c r="C35" s="43"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="42"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="44"/>
       <c r="F35" s="15">
         <v>2</v>
       </c>
-      <c r="G35" s="36"/>
-      <c r="H35" s="42"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="39"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A36" s="28"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="41"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="31"/>
       <c r="B36" s="15">
         <v>2.5</v>
       </c>
-      <c r="C36" s="43"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="42"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="44"/>
       <c r="F36" s="15">
         <v>2.5</v>
       </c>
-      <c r="G36" s="36"/>
-      <c r="H36" s="42"/>
-      <c r="I36" s="43">
+      <c r="G36" s="38"/>
+      <c r="H36" s="44"/>
+      <c r="I36" s="45">
         <v>2</v>
       </c>
-      <c r="J36" s="59" t="s">
+      <c r="J36" s="61" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="29"/>
+    <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="32"/>
       <c r="B37" s="17">
         <v>3</v>
       </c>
-      <c r="C37" s="54"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="55"/>
+      <c r="C37" s="56"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="57"/>
       <c r="F37" s="17">
         <v>3</v>
       </c>
-      <c r="G37" s="40"/>
-      <c r="H37" s="55"/>
-      <c r="I37" s="54"/>
-      <c r="J37" s="60"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A38" s="44" t="s">
+      <c r="G37" s="42"/>
+      <c r="H37" s="57"/>
+      <c r="I37" s="56"/>
+      <c r="J37" s="62"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="46" t="s">
         <v>17</v>
       </c>
       <c r="B38" s="18">
         <v>1.2</v>
       </c>
-      <c r="C38" s="47">
+      <c r="C38" s="49">
         <v>1</v>
       </c>
-      <c r="D38" s="35" t="s">
+      <c r="D38" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="44" t="s">
+      <c r="E38" s="46" t="s">
         <v>13</v>
       </c>
       <c r="F38" s="18">
         <v>1.5</v>
       </c>
-      <c r="G38" s="35" t="s">
+      <c r="G38" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="H38" s="44" t="s">
+      <c r="H38" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="I38" s="47">
+      <c r="I38" s="49">
         <v>1</v>
       </c>
-      <c r="J38" s="35" t="s">
+      <c r="J38" s="37" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A39" s="45"/>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="47"/>
       <c r="B39" s="2">
         <v>1.5</v>
       </c>
-      <c r="C39" s="30"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="45"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="47"/>
       <c r="F39" s="2">
         <v>2</v>
       </c>
-      <c r="G39" s="36"/>
-      <c r="H39" s="45"/>
-      <c r="I39" s="30"/>
-      <c r="J39" s="36"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A40" s="45"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="47"/>
+      <c r="I39" s="28"/>
+      <c r="J39" s="38"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="47"/>
       <c r="B40" s="2">
         <v>1.7</v>
       </c>
-      <c r="C40" s="30"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="45"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="47"/>
       <c r="F40" s="2">
         <v>2.5</v>
       </c>
-      <c r="G40" s="36"/>
-      <c r="H40" s="45"/>
-      <c r="I40" s="30">
+      <c r="G40" s="38"/>
+      <c r="H40" s="47"/>
+      <c r="I40" s="28">
         <v>2</v>
       </c>
-      <c r="J40" s="36"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A41" s="45"/>
+      <c r="J40" s="38"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="47"/>
       <c r="B41" s="2">
         <v>2</v>
       </c>
-      <c r="C41" s="30"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="45"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="47"/>
       <c r="F41" s="2">
         <v>3</v>
       </c>
-      <c r="G41" s="36"/>
-      <c r="H41" s="45"/>
-      <c r="I41" s="30"/>
-      <c r="J41" s="36"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A42" s="45"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="47"/>
+      <c r="I41" s="28"/>
+      <c r="J41" s="38"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="47"/>
       <c r="B42" s="2">
         <v>2.5</v>
       </c>
-      <c r="C42" s="30"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="41" t="s">
+      <c r="C42" s="28"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="43" t="s">
         <v>14</v>
       </c>
       <c r="F42" s="2">
         <v>1.5</v>
       </c>
-      <c r="G42" s="36"/>
-      <c r="H42" s="41" t="s">
+      <c r="G42" s="38"/>
+      <c r="H42" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="I42" s="30">
+      <c r="I42" s="28">
         <v>1</v>
       </c>
-      <c r="J42" s="36"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A43" s="45"/>
+      <c r="J42" s="38"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="47"/>
       <c r="B43" s="2">
         <v>3</v>
       </c>
-      <c r="C43" s="30"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="41"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="43"/>
       <c r="F43" s="2">
         <v>2</v>
       </c>
-      <c r="G43" s="36"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="30"/>
-      <c r="J43" s="36"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A44" s="45"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="28"/>
+      <c r="J43" s="38"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="47"/>
       <c r="B44" s="2">
         <v>1.2</v>
       </c>
-      <c r="C44" s="30">
+      <c r="C44" s="28">
         <v>2</v>
       </c>
-      <c r="D44" s="36"/>
-      <c r="E44" s="41"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="43"/>
       <c r="F44" s="2">
         <v>2.5</v>
       </c>
-      <c r="G44" s="36"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="30">
+      <c r="G44" s="38"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="28">
         <v>2</v>
       </c>
-      <c r="J44" s="36"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A45" s="45"/>
+      <c r="J44" s="38"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="47"/>
       <c r="B45" s="2">
         <v>1.5</v>
       </c>
-      <c r="C45" s="30"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="41"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="43"/>
       <c r="F45" s="2">
         <v>3</v>
       </c>
-      <c r="G45" s="36"/>
-      <c r="H45" s="41"/>
-      <c r="I45" s="30"/>
-      <c r="J45" s="36"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A46" s="45"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="43"/>
+      <c r="I45" s="28"/>
+      <c r="J45" s="38"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="47"/>
       <c r="B46" s="2">
         <v>1.7</v>
       </c>
-      <c r="C46" s="30"/>
-      <c r="D46" s="36"/>
-      <c r="E46" s="41" t="s">
+      <c r="C46" s="28"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="43" t="s">
         <v>15</v>
       </c>
       <c r="F46" s="2">
         <v>1.5</v>
       </c>
-      <c r="G46" s="36"/>
-      <c r="H46" s="41" t="s">
+      <c r="G46" s="38"/>
+      <c r="H46" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="I46" s="30">
+      <c r="I46" s="28">
         <v>1</v>
       </c>
-      <c r="J46" s="36"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A47" s="45"/>
+      <c r="J46" s="38"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="47"/>
       <c r="B47" s="2">
         <v>2</v>
       </c>
-      <c r="C47" s="30"/>
-      <c r="D47" s="36"/>
-      <c r="E47" s="41"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="38"/>
+      <c r="E47" s="43"/>
       <c r="F47" s="2">
         <v>2</v>
       </c>
-      <c r="G47" s="36"/>
-      <c r="H47" s="41"/>
-      <c r="I47" s="30"/>
-      <c r="J47" s="36"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A48" s="45"/>
+      <c r="G47" s="38"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="28"/>
+      <c r="J47" s="38"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="47"/>
       <c r="B48" s="2">
         <v>2.5</v>
       </c>
-      <c r="C48" s="30"/>
-      <c r="D48" s="36"/>
-      <c r="E48" s="41"/>
+      <c r="C48" s="28"/>
+      <c r="D48" s="38"/>
+      <c r="E48" s="43"/>
       <c r="F48" s="2">
         <v>2.5</v>
       </c>
-      <c r="G48" s="36"/>
-      <c r="H48" s="41"/>
-      <c r="I48" s="30">
+      <c r="G48" s="38"/>
+      <c r="H48" s="43"/>
+      <c r="I48" s="28">
         <v>2</v>
       </c>
-      <c r="J48" s="36"/>
-    </row>
-    <row r="49" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="46"/>
+      <c r="J48" s="38"/>
+    </row>
+    <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="48"/>
       <c r="B49" s="20">
         <v>3</v>
       </c>
-      <c r="C49" s="31"/>
-      <c r="D49" s="40"/>
-      <c r="E49" s="48"/>
+      <c r="C49" s="33"/>
+      <c r="D49" s="42"/>
+      <c r="E49" s="50"/>
       <c r="F49" s="20">
         <v>3</v>
       </c>
-      <c r="G49" s="40"/>
-      <c r="H49" s="48"/>
-      <c r="I49" s="31"/>
-      <c r="J49" s="40"/>
+      <c r="G49" s="42"/>
+      <c r="H49" s="50"/>
+      <c r="I49" s="33"/>
+      <c r="J49" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="79">
@@ -9944,27 +10274,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E5ED226-BA1A-41A1-A969-1FDD4768045A}">
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView zoomScale="117" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+      <selection activeCell="C39" sqref="C39:G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="1"/>
     <col min="4" max="4" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.54296875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7265625" style="1"/>
+    <col min="5" max="5" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>32</v>
       </c>
@@ -9990,11 +10320,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="61">
+      <c r="B2" s="63">
         <v>1</v>
       </c>
       <c r="C2" s="26">
@@ -10010,9 +10340,9 @@
         <v>7.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="30"/>
-      <c r="B3" s="62"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="28"/>
+      <c r="B3" s="64"/>
       <c r="C3" s="26">
         <v>2</v>
       </c>
@@ -10032,9 +10362,9 @@
         <v>2.1970000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="30"/>
-      <c r="B4" s="62"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="28"/>
+      <c r="B4" s="64"/>
       <c r="C4" s="26">
         <v>3</v>
       </c>
@@ -10054,9 +10384,9 @@
         <v>3.1779999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="30"/>
-      <c r="B5" s="63"/>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="28"/>
+      <c r="B5" s="65"/>
       <c r="C5" s="26">
         <v>4</v>
       </c>
@@ -10076,9 +10406,9 @@
         <v>7.1150000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="30"/>
-      <c r="B6" s="61">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="28"/>
+      <c r="B6" s="63">
         <v>2</v>
       </c>
       <c r="C6" s="2">
@@ -10094,9 +10424,9 @@
         <v>5.8000000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="30"/>
-      <c r="B7" s="62"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="28"/>
+      <c r="B7" s="64"/>
       <c r="C7" s="2">
         <v>2</v>
       </c>
@@ -10110,9 +10440,9 @@
         <v>0.184</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="30"/>
-      <c r="B8" s="62"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="28"/>
+      <c r="B8" s="64"/>
       <c r="C8" s="2">
         <v>3</v>
       </c>
@@ -10132,9 +10462,9 @@
         <v>2.302</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="30"/>
-      <c r="B9" s="63"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="28"/>
+      <c r="B9" s="65"/>
       <c r="C9" s="2">
         <v>4</v>
       </c>
@@ -10154,9 +10484,9 @@
         <v>4.5579999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="30"/>
-      <c r="B10" s="61">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="28"/>
+      <c r="B10" s="63">
         <v>3</v>
       </c>
       <c r="C10" s="26">
@@ -10172,9 +10502,9 @@
         <v>6.3E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="30"/>
-      <c r="B11" s="62"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="28"/>
+      <c r="B11" s="64"/>
       <c r="C11" s="26">
         <v>2</v>
       </c>
@@ -10188,9 +10518,9 @@
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="30"/>
-      <c r="B12" s="62"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
+      <c r="B12" s="64"/>
       <c r="C12" s="26">
         <v>3</v>
       </c>
@@ -10204,9 +10534,9 @@
         <v>0.73899999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="30"/>
-      <c r="B13" s="63"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="28"/>
+      <c r="B13" s="65"/>
       <c r="C13" s="26">
         <v>4</v>
       </c>
@@ -10220,9 +10550,9 @@
         <v>3.0089999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="30"/>
-      <c r="B14" s="61">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="28"/>
+      <c r="B14" s="63">
         <v>4</v>
       </c>
       <c r="C14" s="2">
@@ -10238,9 +10568,9 @@
         <v>5.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="30"/>
-      <c r="B15" s="62"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+      <c r="B15" s="64"/>
       <c r="C15" s="2">
         <v>2</v>
       </c>
@@ -10254,9 +10584,9 @@
         <v>0.184</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="30"/>
-      <c r="B16" s="62"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="28"/>
+      <c r="B16" s="64"/>
       <c r="C16" s="2">
         <v>3</v>
       </c>
@@ -10270,9 +10600,9 @@
         <v>0.76300000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="30"/>
-      <c r="B17" s="63"/>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="28"/>
+      <c r="B17" s="65"/>
       <c r="C17" s="2">
         <v>4</v>
       </c>
@@ -10286,11 +10616,11 @@
         <v>3.016</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="65" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="61">
+      <c r="B18" s="63">
         <v>1</v>
       </c>
       <c r="C18" s="26" t="s">
@@ -10312,9 +10642,9 @@
         <v>1.9159999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="64"/>
-      <c r="B19" s="62"/>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="28"/>
+      <c r="B19" s="64"/>
       <c r="C19" s="26"/>
       <c r="D19" s="26"/>
       <c r="E19" s="26"/>
@@ -10322,9 +10652,9 @@
       <c r="G19" s="26"/>
       <c r="H19" s="26"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="64"/>
-      <c r="B20" s="62"/>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="28"/>
+      <c r="B20" s="64"/>
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
       <c r="E20" s="26"/>
@@ -10332,9 +10662,9 @@
       <c r="G20" s="26"/>
       <c r="H20" s="26"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="64"/>
-      <c r="B21" s="63"/>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="28"/>
+      <c r="B21" s="65"/>
       <c r="C21" s="26"/>
       <c r="D21" s="26"/>
       <c r="E21" s="26"/>
@@ -10342,9 +10672,9 @@
       <c r="G21" s="26"/>
       <c r="H21" s="26"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="64"/>
-      <c r="B22" s="61">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="28"/>
+      <c r="B22" s="63">
         <v>2</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -10366,9 +10696,9 @@
         <v>1.9139999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="64"/>
-      <c r="B23" s="62"/>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="28"/>
+      <c r="B23" s="64"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -10376,9 +10706,9 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="64"/>
-      <c r="B24" s="62"/>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="28"/>
+      <c r="B24" s="64"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -10386,9 +10716,9 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="64"/>
-      <c r="B25" s="63"/>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="28"/>
+      <c r="B25" s="65"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -10396,9 +10726,9 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="64"/>
-      <c r="B26" s="61">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="28"/>
+      <c r="B26" s="63">
         <v>3</v>
       </c>
       <c r="C26" s="26" t="s">
@@ -10414,9 +10744,9 @@
         <v>0.39600000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="64"/>
-      <c r="B27" s="62"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="28"/>
+      <c r="B27" s="64"/>
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
       <c r="E27" s="26"/>
@@ -10424,9 +10754,9 @@
       <c r="G27" s="26"/>
       <c r="H27" s="26"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="64"/>
-      <c r="B28" s="62"/>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="28"/>
+      <c r="B28" s="64"/>
       <c r="C28" s="26"/>
       <c r="D28" s="26"/>
       <c r="E28" s="26"/>
@@ -10434,9 +10764,9 @@
       <c r="G28" s="26"/>
       <c r="H28" s="26"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="64"/>
-      <c r="B29" s="63"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="28"/>
+      <c r="B29" s="65"/>
       <c r="C29" s="26"/>
       <c r="D29" s="26"/>
       <c r="E29" s="26"/>
@@ -10444,9 +10774,9 @@
       <c r="G29" s="26"/>
       <c r="H29" s="26"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="64"/>
-      <c r="B30" s="61">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="28"/>
+      <c r="B30" s="63">
         <v>4</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -10462,9 +10792,9 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="64"/>
-      <c r="B31" s="62"/>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="28"/>
+      <c r="B31" s="64"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -10472,9 +10802,9 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="64"/>
-      <c r="B32" s="62"/>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="28"/>
+      <c r="B32" s="64"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -10482,9 +10812,9 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="64"/>
-      <c r="B33" s="63"/>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="28"/>
+      <c r="B33" s="65"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -10492,11 +10822,11 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="64" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="61">
+      <c r="B34" s="63">
         <v>1</v>
       </c>
       <c r="C34" s="26" t="s">
@@ -10518,9 +10848,9 @@
         <v>1.732</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="64"/>
-      <c r="B35" s="62"/>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="28"/>
+      <c r="B35" s="64"/>
       <c r="C35" s="26" t="s">
         <v>44</v>
       </c>
@@ -10540,9 +10870,9 @@
         <v>2.431</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="64"/>
-      <c r="B36" s="62"/>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="28"/>
+      <c r="B36" s="64"/>
       <c r="C36" s="26" t="s">
         <v>45</v>
       </c>
@@ -10562,9 +10892,9 @@
         <v>2.35</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" s="64"/>
-      <c r="B37" s="63"/>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="28"/>
+      <c r="B37" s="65"/>
       <c r="C37" s="26" t="s">
         <v>46</v>
       </c>
@@ -10584,9 +10914,9 @@
         <v>4.5430000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A38" s="64"/>
-      <c r="B38" s="61">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="28"/>
+      <c r="B38" s="63">
         <v>2</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -10602,9 +10932,9 @@
         <v>0.22600000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" s="64"/>
-      <c r="B39" s="62"/>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="28"/>
+      <c r="B39" s="64"/>
       <c r="C39" s="2" t="s">
         <v>44</v>
       </c>
@@ -10624,9 +10954,9 @@
         <v>2.2989999999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A40" s="64"/>
-      <c r="B40" s="62"/>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="28"/>
+      <c r="B40" s="64"/>
       <c r="C40" s="2" t="s">
         <v>45</v>
       </c>
@@ -10646,9 +10976,9 @@
         <v>2.3109999999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A41" s="64"/>
-      <c r="B41" s="63"/>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="28"/>
+      <c r="B41" s="65"/>
       <c r="C41" s="2" t="s">
         <v>46</v>
       </c>
@@ -10668,9 +10998,9 @@
         <v>4.5709999999999997</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A42" s="64"/>
-      <c r="B42" s="61">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="28"/>
+      <c r="B42" s="63">
         <v>3</v>
       </c>
       <c r="C42" s="26" t="s">
@@ -10686,9 +11016,9 @@
         <v>0.24199999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A43" s="64"/>
-      <c r="B43" s="62"/>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="28"/>
+      <c r="B43" s="64"/>
       <c r="C43" s="26" t="s">
         <v>44</v>
       </c>
@@ -10702,9 +11032,9 @@
         <v>0.78100000000000003</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A44" s="64"/>
-      <c r="B44" s="62"/>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="28"/>
+      <c r="B44" s="64"/>
       <c r="C44" s="26" t="s">
         <v>45</v>
       </c>
@@ -10724,9 +11054,9 @@
         <v>2.343</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A45" s="64"/>
-      <c r="B45" s="63"/>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="28"/>
+      <c r="B45" s="65"/>
       <c r="C45" s="26" t="s">
         <v>46</v>
       </c>
@@ -10746,9 +11076,9 @@
         <v>4.5750000000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A46" s="64"/>
-      <c r="B46" s="61">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="28"/>
+      <c r="B46" s="63">
         <v>4</v>
       </c>
       <c r="C46" s="2" t="s">
@@ -10764,9 +11094,9 @@
         <v>0.23799999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A47" s="64"/>
-      <c r="B47" s="62"/>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="28"/>
+      <c r="B47" s="64"/>
       <c r="C47" s="2" t="s">
         <v>44</v>
       </c>
@@ -10780,9 +11110,9 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A48" s="64"/>
-      <c r="B48" s="62"/>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="28"/>
+      <c r="B48" s="64"/>
       <c r="C48" s="2" t="s">
         <v>45</v>
       </c>
@@ -10796,9 +11126,9 @@
         <v>0.79700000000000004</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A49" s="64"/>
-      <c r="B49" s="63"/>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="28"/>
+      <c r="B49" s="65"/>
       <c r="C49" s="2" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
Used webcam on Go1 to record video
</commit_message>
<xml_diff>
--- a/detect_methods_comp.xlsx
+++ b/detect_methods_comp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iwaya\Escritorio\Code\FaceRecogServer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABADF2DA-842B-4ECF-AE0B-E4DB6A229E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369FED87-8541-4031-9F45-51113A03B670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resultados" sheetId="6" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="79">
   <si>
     <t>Up Sampling [dlib.get_frontal_face_detector()]</t>
   </si>
@@ -184,21 +184,6 @@
     <t>4, 2</t>
   </si>
   <si>
-    <t>Reconocimiento facial</t>
-  </si>
-  <si>
-    <t>Si*</t>
-  </si>
-  <si>
-    <t>0.38 segundos</t>
-  </si>
-  <si>
-    <t>11 segundos</t>
-  </si>
-  <si>
-    <t>1.5 segundos</t>
-  </si>
-  <si>
     <t>Número de rostros en escena</t>
   </si>
   <si>
@@ -206,15 +191,6 @@
   </si>
   <si>
     <t>1856x800</t>
-  </si>
-  <si>
-    <t>Promedio detección facial y envió del face chip</t>
-  </si>
-  <si>
-    <t>Promedio de extracción de características y reconocimiento facial</t>
-  </si>
-  <si>
-    <t>Promedio envió imagezmq</t>
   </si>
   <si>
     <t>1 metro</t>
@@ -235,19 +211,73 @@
     <t>928x400</t>
   </si>
   <si>
-    <t>*Si la calidad de la imagen transmitida internamente lo permite, en general la calidad de la imagen era muy baja como para hacer FR</t>
+    <t>Detección facial</t>
   </si>
   <si>
-    <t>11.5 segundos</t>
+    <t>1 - 1.5 segundos</t>
   </si>
   <si>
-    <t>1 segundo</t>
+    <t>10 - 11 segundos</t>
   </si>
   <si>
-    <t>0.4 segundos</t>
+    <t>0.38 - 0.40 segundos</t>
   </si>
   <si>
-    <t>928x400 (re-escalado por 2 en placa receptora interna)</t>
+    <t>0.37 - 0.4 segundos</t>
+  </si>
+  <si>
+    <t>Tiempo envió imagezmq</t>
+  </si>
+  <si>
+    <t>Tiempo de extracción de características y reconocimiento facial</t>
+  </si>
+  <si>
+    <t>Tiempo detección facial y envió del face chip</t>
+  </si>
+  <si>
+    <t>11 - 12 segundos</t>
+  </si>
+  <si>
+    <t>Obs</t>
+  </si>
+  <si>
+    <t>La transmisión interna de video es lenta y la mayoría de imágenes posee artefactos debido a la compresión</t>
+  </si>
+  <si>
+    <t>La transmisión de video es estable y disminuye la cantidad de artefactos, eventualmente no es posible detectar rostros a mayor distancia debido al tamaño de la imagen</t>
+  </si>
+  <si>
+    <t>FPS transmisión interna</t>
+  </si>
+  <si>
+    <t>El tamaño de la imagen es muy pequeño para realizar detección facial</t>
+  </si>
+  <si>
+    <t>464x200</t>
+  </si>
+  <si>
+    <t>232x100</t>
+  </si>
+  <si>
+    <t>116x50</t>
+  </si>
+  <si>
+    <t>464x200 (x4 con resize)</t>
+  </si>
+  <si>
+    <t>1.53 - 1.8 segundos</t>
+  </si>
+  <si>
+    <t>0.4 - 0.44 segundos</t>
+  </si>
+  <si>
+    <t>Como es de esperar, la función resize de OpenCV tarda en procesar (ver Resize (OpenCV))</t>
+  </si>
+  <si>
+    <t>0.5 - 0.54 segundos</t>
+  </si>
+  <si>
+    <t>El tamaño de la imagen es muy pequeño para realizar detección facial,  la tasa de transmisión no mejora (fps)</t>
   </si>
 </sst>
 </file>
@@ -271,7 +301,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,6 +359,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -591,7 +627,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -671,14 +707,8 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -787,6 +817,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7901,275 +7946,615 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD554FA1-10E3-4A88-8A1D-54AF58A25FC5}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10:I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="56.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" style="1" customWidth="1"/>
+    <col min="2" max="3" width="15.6328125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="17" style="1" customWidth="1"/>
+    <col min="6" max="6" width="29.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="32.54296875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7265625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="41.54296875" style="66" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="67" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="68" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="68" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="67" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="67" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="67" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="67" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="65" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="27">
+        <v>1</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="27">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="64" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="64"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="E4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="64"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="27" t="s">
+      <c r="E5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="64"/>
+    </row>
+    <row r="6" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="27"/>
+      <c r="B6" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="28">
+      <c r="C6" s="27">
+        <v>22.32</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I6" s="64" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="F7" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="G7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="64"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="64"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="64"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="27">
+        <v>23.43</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="64" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" s="64"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="64"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="64"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="27"/>
+      <c r="B14" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="27">
+        <v>23.42</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14" s="64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" s="64"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" s="64"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17" s="64"/>
+    </row>
+    <row r="18" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="27">
+        <v>24</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I18" s="64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19" s="64"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I20" s="64"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I21" s="64"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="27"/>
+      <c r="B22" s="64" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="27">
+        <v>23.43</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="I22" s="64" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="27"/>
+      <c r="B23" s="64"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="F23" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I23" s="64"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="27"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="F24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I24" s="64"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" s="27"/>
+      <c r="B25" s="64"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>64</v>
-      </c>
+      <c r="F25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I25" s="64"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="19">
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="I22:I25"/>
+    <mergeCell ref="A2:A25"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="I18:I21"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B6:B9"/>
+    <mergeCell ref="I2:I5"/>
+    <mergeCell ref="I6:I9"/>
     <mergeCell ref="B10:B13"/>
-    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="I10:I13"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="I14:I17"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="C14:C17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8180,26 +8565,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6706964-F93E-4934-BEB2-8D6878ECF54C}">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView zoomScale="103" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView zoomScale="93" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="12" width="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>27</v>
       </c>
@@ -8227,7 +8612,7 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
@@ -8271,7 +8656,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -8319,7 +8704,7 @@
         <v>1.1792592592592592</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -8367,7 +8752,7 @@
         <v>3.2364197530864196</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -8415,7 +8800,7 @@
         <v>6.2976543209876548</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -8463,7 +8848,7 @@
         <v>10.856419753086421</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -8511,7 +8896,7 @@
         <v>16.636172839506173</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -8574,24 +8959,24 @@
       <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="44.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="12" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="9.140625" style="1"/>
+    <col min="16" max="17" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>27</v>
       </c>
@@ -8611,7 +8996,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -8655,7 +9040,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>0</v>
       </c>
@@ -8703,7 +9088,7 @@
         <v>1.2112345679012346</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -8751,7 +9136,7 @@
         <v>3.3197530864197526</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>2</v>
       </c>
@@ -8799,7 +9184,7 @@
         <v>11.808518518518518</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>3</v>
       </c>
@@ -8847,7 +9232,7 @@
         <v>45.358148148148153</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -8895,7 +9280,7 @@
         <v>178.80925925925925</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>5</v>
       </c>
@@ -8943,19 +9328,19 @@
         <v>728.60370370370367</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D13" s="1"/>
     </row>
   </sheetData>
@@ -8973,23 +9358,23 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="42.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" customWidth="1"/>
+    <col min="8" max="8" width="42.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>27</v>
       </c>
@@ -9017,7 +9402,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>21</v>
       </c>
@@ -9062,7 +9447,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
@@ -9111,7 +9496,7 @@
         <v>16.113456790123458</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>14</v>
       </c>
@@ -9160,7 +9545,7 @@
         <v>20.674814814814816</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
@@ -9224,969 +9609,969 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="14" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" style="14" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="8.54296875" style="14" customWidth="1"/>
     <col min="8" max="8" width="15" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5703125" style="14" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="14" customWidth="1"/>
+    <col min="9" max="9" width="6.54296875" style="14" customWidth="1"/>
+    <col min="10" max="10" width="9.1796875" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="58"/>
+      <c r="C1" s="56"/>
       <c r="D1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="59" t="s">
+      <c r="E1" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="58"/>
+      <c r="F1" s="56"/>
       <c r="G1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="59" t="s">
+      <c r="H1" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="58"/>
+      <c r="I1" s="56"/>
       <c r="J1" s="25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="28" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="16">
         <v>1.2</v>
       </c>
-      <c r="C2" s="51">
+      <c r="C2" s="49">
         <v>1</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="28" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="16">
         <v>1.5</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="30" t="s">
+      <c r="H2" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="51">
+      <c r="I2" s="49">
         <v>1</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="J2" s="32" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="29"/>
       <c r="B3" s="15">
         <v>1.5</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="31"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="29"/>
       <c r="F3" s="15">
         <v>2</v>
       </c>
-      <c r="G3" s="35"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="35"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="33"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="29"/>
       <c r="B4" s="15">
         <v>1.7</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="31"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="29"/>
       <c r="F4" s="15">
         <v>2.5</v>
       </c>
-      <c r="G4" s="35"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="45">
+      <c r="G4" s="33"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="43">
         <v>2</v>
       </c>
-      <c r="J4" s="35"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
+      <c r="J4" s="33"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="29"/>
       <c r="B5" s="15">
         <v>2</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="31"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="29"/>
       <c r="F5" s="15">
         <v>3</v>
       </c>
-      <c r="G5" s="35"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="35"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="33"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="29"/>
       <c r="B6" s="15">
         <v>2.5</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="44" t="s">
+      <c r="C6" s="43"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="42" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="15">
         <v>1.5</v>
       </c>
-      <c r="G6" s="35"/>
-      <c r="H6" s="44" t="s">
+      <c r="G6" s="33"/>
+      <c r="H6" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="45">
+      <c r="I6" s="43">
         <v>1</v>
       </c>
-      <c r="J6" s="35"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+      <c r="J6" s="33"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="29"/>
       <c r="B7" s="15">
         <v>3</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="44"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="42"/>
       <c r="F7" s="15">
         <v>2</v>
       </c>
-      <c r="G7" s="35"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="35"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="33"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="29"/>
       <c r="B8" s="15">
         <v>1.2</v>
       </c>
-      <c r="C8" s="45">
+      <c r="C8" s="43">
         <v>2</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="44"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="42"/>
       <c r="F8" s="15">
         <v>2.5</v>
       </c>
-      <c r="G8" s="35"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="45">
+      <c r="G8" s="33"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="43">
         <v>2</v>
       </c>
-      <c r="J8" s="35"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
+      <c r="J8" s="33"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="29"/>
       <c r="B9" s="15">
         <v>1.5</v>
       </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="44"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="42"/>
       <c r="F9" s="15">
         <v>3</v>
       </c>
-      <c r="G9" s="35"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="35"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="33"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="29"/>
       <c r="B10" s="15">
         <v>1.7</v>
       </c>
-      <c r="C10" s="45"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="44" t="s">
+      <c r="C10" s="43"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="42" t="s">
         <v>15</v>
       </c>
       <c r="F10" s="15">
         <v>1.5</v>
       </c>
-      <c r="G10" s="35"/>
-      <c r="H10" s="44" t="s">
+      <c r="G10" s="33"/>
+      <c r="H10" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="45">
+      <c r="I10" s="43">
         <v>1</v>
       </c>
-      <c r="J10" s="35"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="J10" s="33"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="29"/>
       <c r="B11" s="15">
         <v>2</v>
       </c>
-      <c r="C11" s="45"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="44"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="42"/>
       <c r="F11" s="15">
         <v>2</v>
       </c>
-      <c r="G11" s="35"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="35"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="33"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="29"/>
       <c r="B12" s="15">
         <v>2.5</v>
       </c>
-      <c r="C12" s="45"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="44"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="42"/>
       <c r="F12" s="15">
         <v>2.5</v>
       </c>
-      <c r="G12" s="35"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="45">
+      <c r="G12" s="33"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="43">
         <v>2</v>
       </c>
-      <c r="J12" s="35"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="32"/>
+      <c r="J12" s="33"/>
+    </row>
+    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="30"/>
       <c r="B13" s="17">
         <v>3</v>
       </c>
-      <c r="C13" s="56"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="57"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="55"/>
       <c r="F13" s="17">
         <v>3</v>
       </c>
-      <c r="G13" s="36"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="56"/>
-      <c r="J13" s="36"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="46" t="s">
+      <c r="G13" s="34"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="34"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="44" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="18">
         <v>1.2</v>
       </c>
-      <c r="C14" s="49">
+      <c r="C14" s="47">
         <v>1</v>
       </c>
-      <c r="D14" s="37" t="s">
+      <c r="D14" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="46" t="s">
+      <c r="E14" s="44" t="s">
         <v>13</v>
       </c>
       <c r="F14" s="18">
         <v>1.5</v>
       </c>
-      <c r="G14" s="34" t="s">
+      <c r="G14" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="H14" s="46" t="s">
+      <c r="H14" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="49">
+      <c r="I14" s="47">
         <v>1</v>
       </c>
-      <c r="J14" s="34" t="s">
+      <c r="J14" s="32" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="45"/>
       <c r="B15" s="2">
         <v>1.5</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="47"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="45"/>
       <c r="F15" s="2">
         <v>2</v>
       </c>
-      <c r="G15" s="35"/>
-      <c r="H15" s="47"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="35"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="33"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="45"/>
       <c r="B16" s="2">
         <v>1.7</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="47"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="45"/>
       <c r="F16" s="2">
         <v>2.5</v>
       </c>
-      <c r="G16" s="35"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="28">
+      <c r="G16" s="33"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="27">
         <v>2</v>
       </c>
-      <c r="J16" s="35"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
+      <c r="J16" s="33"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="45"/>
       <c r="B17" s="2">
         <v>2</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="47"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="45"/>
       <c r="F17" s="2">
         <v>3</v>
       </c>
-      <c r="G17" s="35"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="35"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="33"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="45"/>
       <c r="B18" s="2">
         <v>2.5</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="40" t="s">
+      <c r="C18" s="27"/>
+      <c r="D18" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="43" t="s">
+      <c r="E18" s="41" t="s">
         <v>14</v>
       </c>
       <c r="F18" s="2">
         <v>1.5</v>
       </c>
-      <c r="G18" s="35"/>
-      <c r="H18" s="43" t="s">
+      <c r="G18" s="33"/>
+      <c r="H18" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="I18" s="28">
+      <c r="I18" s="27">
         <v>1</v>
       </c>
-      <c r="J18" s="35"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
+      <c r="J18" s="33"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="45"/>
       <c r="B19" s="2">
         <v>3</v>
       </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="43"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="41"/>
       <c r="F19" s="2">
         <v>2</v>
       </c>
-      <c r="G19" s="35"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="35"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="33"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="45"/>
       <c r="B20" s="2">
         <v>1.2</v>
       </c>
-      <c r="C20" s="28">
+      <c r="C20" s="27">
         <v>2</v>
       </c>
       <c r="D20" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="43"/>
+      <c r="E20" s="41"/>
       <c r="F20" s="2">
         <v>2.5</v>
       </c>
-      <c r="G20" s="35"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="28">
+      <c r="G20" s="33"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="27">
         <v>2</v>
       </c>
-      <c r="J20" s="35"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
+      <c r="J20" s="33"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="45"/>
       <c r="B21" s="2">
         <v>1.5</v>
       </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="40" t="s">
+      <c r="C21" s="27"/>
+      <c r="D21" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="43"/>
+      <c r="E21" s="41"/>
       <c r="F21" s="2">
         <v>3</v>
       </c>
-      <c r="G21" s="35"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="35"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="33"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" s="45"/>
       <c r="B22" s="2">
         <v>1.7</v>
       </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="43" t="s">
+      <c r="C22" s="27"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="41" t="s">
         <v>15</v>
       </c>
       <c r="F22" s="2">
         <v>1.5</v>
       </c>
-      <c r="G22" s="35"/>
-      <c r="H22" s="43" t="s">
+      <c r="G22" s="33"/>
+      <c r="H22" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="I22" s="28">
+      <c r="I22" s="27">
         <v>1</v>
       </c>
-      <c r="J22" s="35"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="47"/>
+      <c r="J22" s="33"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" s="45"/>
       <c r="B23" s="2">
         <v>2</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="43"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="41"/>
       <c r="F23" s="2">
         <v>2</v>
       </c>
-      <c r="G23" s="35"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="35"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="33"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" s="45"/>
       <c r="B24" s="2">
         <v>2.5</v>
       </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="43"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="41"/>
       <c r="F24" s="2">
         <v>2.5</v>
       </c>
-      <c r="G24" s="35"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="28">
+      <c r="G24" s="33"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="27">
         <v>2</v>
       </c>
-      <c r="J24" s="35"/>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="48"/>
+      <c r="J24" s="33"/>
+    </row>
+    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="46"/>
       <c r="B25" s="20">
         <v>3</v>
       </c>
-      <c r="C25" s="33"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="50"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="48"/>
       <c r="F25" s="20">
         <v>3</v>
       </c>
-      <c r="G25" s="36"/>
-      <c r="H25" s="50"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="36"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="30" t="s">
+      <c r="G25" s="34"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="34"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" s="28" t="s">
         <v>18</v>
       </c>
       <c r="B26" s="16">
         <v>1.2</v>
       </c>
-      <c r="C26" s="51">
+      <c r="C26" s="49">
         <v>1</v>
       </c>
-      <c r="D26" s="37" t="s">
+      <c r="D26" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="30" t="s">
+      <c r="E26" s="28" t="s">
         <v>13</v>
       </c>
       <c r="F26" s="16">
         <v>1.5</v>
       </c>
-      <c r="G26" s="37" t="s">
+      <c r="G26" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="H26" s="52" t="s">
+      <c r="H26" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I26" s="54">
+      <c r="I26" s="52">
         <v>1</v>
       </c>
-      <c r="J26" s="34" t="s">
+      <c r="J26" s="32" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" s="29"/>
       <c r="B27" s="15">
         <v>1.5</v>
       </c>
-      <c r="C27" s="45"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="31"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="29"/>
       <c r="F27" s="15">
         <v>2</v>
       </c>
-      <c r="G27" s="38"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="55"/>
-      <c r="J27" s="35"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="53"/>
+      <c r="J27" s="33"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" s="29"/>
       <c r="B28" s="15">
         <v>1.7</v>
       </c>
-      <c r="C28" s="45"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="31"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="29"/>
       <c r="F28" s="15">
         <v>2.5</v>
       </c>
-      <c r="G28" s="38"/>
-      <c r="H28" s="53"/>
-      <c r="I28" s="55">
+      <c r="G28" s="36"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="53">
         <v>2</v>
       </c>
-      <c r="J28" s="35"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="31"/>
+      <c r="J28" s="33"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" s="29"/>
       <c r="B29" s="15">
         <v>2</v>
       </c>
-      <c r="C29" s="45"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="31"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="29"/>
       <c r="F29" s="15">
         <v>3</v>
       </c>
-      <c r="G29" s="38"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="35"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="31"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="33"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" s="29"/>
       <c r="B30" s="15">
         <v>2.5</v>
       </c>
-      <c r="C30" s="45"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="44" t="s">
+      <c r="C30" s="43"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="42" t="s">
         <v>14</v>
       </c>
       <c r="F30" s="15">
         <v>1.5</v>
       </c>
-      <c r="G30" s="39"/>
-      <c r="H30" s="44" t="s">
+      <c r="G30" s="37"/>
+      <c r="H30" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="I30" s="45">
+      <c r="I30" s="43">
         <v>1</v>
       </c>
-      <c r="J30" s="35"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
+      <c r="J30" s="33"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31" s="29"/>
       <c r="B31" s="15">
         <v>3</v>
       </c>
-      <c r="C31" s="45"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="44"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="42"/>
       <c r="F31" s="15">
         <v>2</v>
       </c>
       <c r="G31" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="H31" s="44"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="35"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="43"/>
+      <c r="J31" s="33"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32" s="29"/>
       <c r="B32" s="15">
         <v>1.2</v>
       </c>
-      <c r="C32" s="45">
+      <c r="C32" s="43">
         <v>2</v>
       </c>
-      <c r="D32" s="38"/>
-      <c r="E32" s="44"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="42"/>
       <c r="F32" s="15">
         <v>2.5</v>
       </c>
-      <c r="G32" s="60" t="s">
+      <c r="G32" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="H32" s="44"/>
-      <c r="I32" s="45">
+      <c r="H32" s="42"/>
+      <c r="I32" s="43">
         <v>2</v>
       </c>
-      <c r="J32" s="35"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="31"/>
+      <c r="J32" s="33"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33" s="29"/>
       <c r="B33" s="15">
         <v>1.5</v>
       </c>
-      <c r="C33" s="45"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="44"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="42"/>
       <c r="F33" s="15">
         <v>3</v>
       </c>
-      <c r="G33" s="38"/>
-      <c r="H33" s="44"/>
-      <c r="I33" s="45"/>
-      <c r="J33" s="35"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="31"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="42"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="33"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A34" s="29"/>
       <c r="B34" s="15">
         <v>1.7</v>
       </c>
-      <c r="C34" s="45"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="44" t="s">
+      <c r="C34" s="43"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="42" t="s">
         <v>15</v>
       </c>
       <c r="F34" s="15">
         <v>1.5</v>
       </c>
-      <c r="G34" s="38"/>
-      <c r="H34" s="44" t="s">
+      <c r="G34" s="36"/>
+      <c r="H34" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="I34" s="45">
+      <c r="I34" s="43">
         <v>1</v>
       </c>
-      <c r="J34" s="35"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="31"/>
+      <c r="J34" s="33"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A35" s="29"/>
       <c r="B35" s="15">
         <v>2</v>
       </c>
-      <c r="C35" s="45"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="44"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="42"/>
       <c r="F35" s="15">
         <v>2</v>
       </c>
-      <c r="G35" s="38"/>
-      <c r="H35" s="44"/>
-      <c r="I35" s="45"/>
-      <c r="J35" s="41"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="31"/>
+      <c r="G35" s="36"/>
+      <c r="H35" s="42"/>
+      <c r="I35" s="43"/>
+      <c r="J35" s="39"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A36" s="29"/>
       <c r="B36" s="15">
         <v>2.5</v>
       </c>
-      <c r="C36" s="45"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="44"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="42"/>
       <c r="F36" s="15">
         <v>2.5</v>
       </c>
-      <c r="G36" s="38"/>
-      <c r="H36" s="44"/>
-      <c r="I36" s="45">
+      <c r="G36" s="36"/>
+      <c r="H36" s="42"/>
+      <c r="I36" s="43">
         <v>2</v>
       </c>
-      <c r="J36" s="61" t="s">
+      <c r="J36" s="59" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="32"/>
+    <row r="37" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="30"/>
       <c r="B37" s="17">
         <v>3</v>
       </c>
-      <c r="C37" s="56"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="57"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="55"/>
       <c r="F37" s="17">
         <v>3</v>
       </c>
-      <c r="G37" s="42"/>
-      <c r="H37" s="57"/>
-      <c r="I37" s="56"/>
-      <c r="J37" s="62"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="46" t="s">
+      <c r="G37" s="40"/>
+      <c r="H37" s="55"/>
+      <c r="I37" s="54"/>
+      <c r="J37" s="60"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38" s="44" t="s">
         <v>17</v>
       </c>
       <c r="B38" s="18">
         <v>1.2</v>
       </c>
-      <c r="C38" s="49">
+      <c r="C38" s="47">
         <v>1</v>
       </c>
-      <c r="D38" s="37" t="s">
+      <c r="D38" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="46" t="s">
+      <c r="E38" s="44" t="s">
         <v>13</v>
       </c>
       <c r="F38" s="18">
         <v>1.5</v>
       </c>
-      <c r="G38" s="37" t="s">
+      <c r="G38" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="H38" s="46" t="s">
+      <c r="H38" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="I38" s="49">
+      <c r="I38" s="47">
         <v>1</v>
       </c>
-      <c r="J38" s="37" t="s">
+      <c r="J38" s="35" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="47"/>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A39" s="45"/>
       <c r="B39" s="2">
         <v>1.5</v>
       </c>
-      <c r="C39" s="28"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="47"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="45"/>
       <c r="F39" s="2">
         <v>2</v>
       </c>
-      <c r="G39" s="38"/>
-      <c r="H39" s="47"/>
-      <c r="I39" s="28"/>
-      <c r="J39" s="38"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="47"/>
+      <c r="G39" s="36"/>
+      <c r="H39" s="45"/>
+      <c r="I39" s="27"/>
+      <c r="J39" s="36"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A40" s="45"/>
       <c r="B40" s="2">
         <v>1.7</v>
       </c>
-      <c r="C40" s="28"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="47"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="45"/>
       <c r="F40" s="2">
         <v>2.5</v>
       </c>
-      <c r="G40" s="38"/>
-      <c r="H40" s="47"/>
-      <c r="I40" s="28">
+      <c r="G40" s="36"/>
+      <c r="H40" s="45"/>
+      <c r="I40" s="27">
         <v>2</v>
       </c>
-      <c r="J40" s="38"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="47"/>
+      <c r="J40" s="36"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A41" s="45"/>
       <c r="B41" s="2">
         <v>2</v>
       </c>
-      <c r="C41" s="28"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="47"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="36"/>
+      <c r="E41" s="45"/>
       <c r="F41" s="2">
         <v>3</v>
       </c>
-      <c r="G41" s="38"/>
-      <c r="H41" s="47"/>
-      <c r="I41" s="28"/>
-      <c r="J41" s="38"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="47"/>
+      <c r="G41" s="36"/>
+      <c r="H41" s="45"/>
+      <c r="I41" s="27"/>
+      <c r="J41" s="36"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A42" s="45"/>
       <c r="B42" s="2">
         <v>2.5</v>
       </c>
-      <c r="C42" s="28"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="43" t="s">
+      <c r="C42" s="27"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="41" t="s">
         <v>14</v>
       </c>
       <c r="F42" s="2">
         <v>1.5</v>
       </c>
-      <c r="G42" s="38"/>
-      <c r="H42" s="43" t="s">
+      <c r="G42" s="36"/>
+      <c r="H42" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="I42" s="28">
+      <c r="I42" s="27">
         <v>1</v>
       </c>
-      <c r="J42" s="38"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="47"/>
+      <c r="J42" s="36"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A43" s="45"/>
       <c r="B43" s="2">
         <v>3</v>
       </c>
-      <c r="C43" s="28"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="43"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="41"/>
       <c r="F43" s="2">
         <v>2</v>
       </c>
-      <c r="G43" s="38"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="28"/>
-      <c r="J43" s="38"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="47"/>
+      <c r="G43" s="36"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="36"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A44" s="45"/>
       <c r="B44" s="2">
         <v>1.2</v>
       </c>
-      <c r="C44" s="28">
+      <c r="C44" s="27">
         <v>2</v>
       </c>
-      <c r="D44" s="38"/>
-      <c r="E44" s="43"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="41"/>
       <c r="F44" s="2">
         <v>2.5</v>
       </c>
-      <c r="G44" s="38"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="28">
+      <c r="G44" s="36"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="27">
         <v>2</v>
       </c>
-      <c r="J44" s="38"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="47"/>
+      <c r="J44" s="36"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A45" s="45"/>
       <c r="B45" s="2">
         <v>1.5</v>
       </c>
-      <c r="C45" s="28"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="43"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="41"/>
       <c r="F45" s="2">
         <v>3</v>
       </c>
-      <c r="G45" s="38"/>
-      <c r="H45" s="43"/>
-      <c r="I45" s="28"/>
-      <c r="J45" s="38"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="47"/>
+      <c r="G45" s="36"/>
+      <c r="H45" s="41"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="36"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A46" s="45"/>
       <c r="B46" s="2">
         <v>1.7</v>
       </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="43" t="s">
+      <c r="C46" s="27"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="41" t="s">
         <v>15</v>
       </c>
       <c r="F46" s="2">
         <v>1.5</v>
       </c>
-      <c r="G46" s="38"/>
-      <c r="H46" s="43" t="s">
+      <c r="G46" s="36"/>
+      <c r="H46" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="I46" s="28">
+      <c r="I46" s="27">
         <v>1</v>
       </c>
-      <c r="J46" s="38"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="47"/>
+      <c r="J46" s="36"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A47" s="45"/>
       <c r="B47" s="2">
         <v>2</v>
       </c>
-      <c r="C47" s="28"/>
-      <c r="D47" s="38"/>
-      <c r="E47" s="43"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="41"/>
       <c r="F47" s="2">
         <v>2</v>
       </c>
-      <c r="G47" s="38"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="28"/>
-      <c r="J47" s="38"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="47"/>
+      <c r="G47" s="36"/>
+      <c r="H47" s="41"/>
+      <c r="I47" s="27"/>
+      <c r="J47" s="36"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A48" s="45"/>
       <c r="B48" s="2">
         <v>2.5</v>
       </c>
-      <c r="C48" s="28"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="43"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="36"/>
+      <c r="E48" s="41"/>
       <c r="F48" s="2">
         <v>2.5</v>
       </c>
-      <c r="G48" s="38"/>
-      <c r="H48" s="43"/>
-      <c r="I48" s="28">
+      <c r="G48" s="36"/>
+      <c r="H48" s="41"/>
+      <c r="I48" s="27">
         <v>2</v>
       </c>
-      <c r="J48" s="38"/>
-    </row>
-    <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="48"/>
+      <c r="J48" s="36"/>
+    </row>
+    <row r="49" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="46"/>
       <c r="B49" s="20">
         <v>3</v>
       </c>
-      <c r="C49" s="33"/>
-      <c r="D49" s="42"/>
-      <c r="E49" s="50"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="40"/>
+      <c r="E49" s="48"/>
       <c r="F49" s="20">
         <v>3</v>
       </c>
-      <c r="G49" s="42"/>
-      <c r="H49" s="50"/>
-      <c r="I49" s="33"/>
-      <c r="J49" s="42"/>
+      <c r="G49" s="40"/>
+      <c r="H49" s="48"/>
+      <c r="I49" s="31"/>
+      <c r="J49" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="79">
@@ -10282,19 +10667,19 @@
       <selection activeCell="C39" sqref="C39:G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="20.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="1"/>
     <col min="4" max="4" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="1"/>
+    <col min="5" max="5" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>32</v>
       </c>
@@ -10320,11 +10705,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="63">
+      <c r="B2" s="61">
         <v>1</v>
       </c>
       <c r="C2" s="26">
@@ -10340,9 +10725,9 @@
         <v>7.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="64"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="27"/>
+      <c r="B3" s="62"/>
       <c r="C3" s="26">
         <v>2</v>
       </c>
@@ -10362,9 +10747,9 @@
         <v>2.1970000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="64"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="27"/>
+      <c r="B4" s="62"/>
       <c r="C4" s="26">
         <v>3</v>
       </c>
@@ -10384,9 +10769,9 @@
         <v>3.1779999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="65"/>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="27"/>
+      <c r="B5" s="63"/>
       <c r="C5" s="26">
         <v>4</v>
       </c>
@@ -10406,9 +10791,9 @@
         <v>7.1150000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="63">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="27"/>
+      <c r="B6" s="61">
         <v>2</v>
       </c>
       <c r="C6" s="2">
@@ -10424,9 +10809,9 @@
         <v>5.8000000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="64"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="27"/>
+      <c r="B7" s="62"/>
       <c r="C7" s="2">
         <v>2</v>
       </c>
@@ -10440,9 +10825,9 @@
         <v>0.184</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="64"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="27"/>
+      <c r="B8" s="62"/>
       <c r="C8" s="2">
         <v>3</v>
       </c>
@@ -10462,9 +10847,9 @@
         <v>2.302</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="65"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="27"/>
+      <c r="B9" s="63"/>
       <c r="C9" s="2">
         <v>4</v>
       </c>
@@ -10484,9 +10869,9 @@
         <v>4.5579999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="63">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="27"/>
+      <c r="B10" s="61">
         <v>3</v>
       </c>
       <c r="C10" s="26">
@@ -10502,9 +10887,9 @@
         <v>6.3E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="64"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="27"/>
+      <c r="B11" s="62"/>
       <c r="C11" s="26">
         <v>2</v>
       </c>
@@ -10518,9 +10903,9 @@
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="64"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="27"/>
+      <c r="B12" s="62"/>
       <c r="C12" s="26">
         <v>3</v>
       </c>
@@ -10534,9 +10919,9 @@
         <v>0.73899999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
-      <c r="B13" s="65"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="27"/>
+      <c r="B13" s="63"/>
       <c r="C13" s="26">
         <v>4</v>
       </c>
@@ -10550,9 +10935,9 @@
         <v>3.0089999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
-      <c r="B14" s="63">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="27"/>
+      <c r="B14" s="61">
         <v>4</v>
       </c>
       <c r="C14" s="2">
@@ -10568,9 +10953,9 @@
         <v>5.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="64"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="27"/>
+      <c r="B15" s="62"/>
       <c r="C15" s="2">
         <v>2</v>
       </c>
@@ -10584,9 +10969,9 @@
         <v>0.184</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-      <c r="B16" s="64"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="27"/>
+      <c r="B16" s="62"/>
       <c r="C16" s="2">
         <v>3</v>
       </c>
@@ -10600,9 +10985,9 @@
         <v>0.76300000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="65"/>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="27"/>
+      <c r="B17" s="63"/>
       <c r="C17" s="2">
         <v>4</v>
       </c>
@@ -10616,11 +11001,11 @@
         <v>3.016</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="63">
+      <c r="B18" s="61">
         <v>1</v>
       </c>
       <c r="C18" s="26" t="s">
@@ -10642,9 +11027,9 @@
         <v>1.9159999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
-      <c r="B19" s="64"/>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="27"/>
+      <c r="B19" s="62"/>
       <c r="C19" s="26"/>
       <c r="D19" s="26"/>
       <c r="E19" s="26"/>
@@ -10652,9 +11037,9 @@
       <c r="G19" s="26"/>
       <c r="H19" s="26"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
-      <c r="B20" s="64"/>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="27"/>
+      <c r="B20" s="62"/>
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
       <c r="E20" s="26"/>
@@ -10662,9 +11047,9 @@
       <c r="G20" s="26"/>
       <c r="H20" s="26"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="28"/>
-      <c r="B21" s="65"/>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="27"/>
+      <c r="B21" s="63"/>
       <c r="C21" s="26"/>
       <c r="D21" s="26"/>
       <c r="E21" s="26"/>
@@ -10672,9 +11057,9 @@
       <c r="G21" s="26"/>
       <c r="H21" s="26"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="28"/>
-      <c r="B22" s="63">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="27"/>
+      <c r="B22" s="61">
         <v>2</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -10696,9 +11081,9 @@
         <v>1.9139999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
-      <c r="B23" s="64"/>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="27"/>
+      <c r="B23" s="62"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -10706,9 +11091,9 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
-      <c r="B24" s="64"/>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="27"/>
+      <c r="B24" s="62"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -10716,9 +11101,9 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="28"/>
-      <c r="B25" s="65"/>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="27"/>
+      <c r="B25" s="63"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -10726,9 +11111,9 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="28"/>
-      <c r="B26" s="63">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="27"/>
+      <c r="B26" s="61">
         <v>3</v>
       </c>
       <c r="C26" s="26" t="s">
@@ -10744,9 +11129,9 @@
         <v>0.39600000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="28"/>
-      <c r="B27" s="64"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="27"/>
+      <c r="B27" s="62"/>
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
       <c r="E27" s="26"/>
@@ -10754,9 +11139,9 @@
       <c r="G27" s="26"/>
       <c r="H27" s="26"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="28"/>
-      <c r="B28" s="64"/>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="27"/>
+      <c r="B28" s="62"/>
       <c r="C28" s="26"/>
       <c r="D28" s="26"/>
       <c r="E28" s="26"/>
@@ -10764,9 +11149,9 @@
       <c r="G28" s="26"/>
       <c r="H28" s="26"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="28"/>
-      <c r="B29" s="65"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="27"/>
+      <c r="B29" s="63"/>
       <c r="C29" s="26"/>
       <c r="D29" s="26"/>
       <c r="E29" s="26"/>
@@ -10774,9 +11159,9 @@
       <c r="G29" s="26"/>
       <c r="H29" s="26"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="28"/>
-      <c r="B30" s="63">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="27"/>
+      <c r="B30" s="61">
         <v>4</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -10792,9 +11177,9 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="28"/>
-      <c r="B31" s="64"/>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="27"/>
+      <c r="B31" s="62"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -10802,9 +11187,9 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="28"/>
-      <c r="B32" s="64"/>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="27"/>
+      <c r="B32" s="62"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -10812,9 +11197,9 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
-      <c r="B33" s="65"/>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="27"/>
+      <c r="B33" s="63"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -10822,11 +11207,11 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="28" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="63">
+      <c r="B34" s="61">
         <v>1</v>
       </c>
       <c r="C34" s="26" t="s">
@@ -10848,9 +11233,9 @@
         <v>1.732</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="28"/>
-      <c r="B35" s="64"/>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="27"/>
+      <c r="B35" s="62"/>
       <c r="C35" s="26" t="s">
         <v>44</v>
       </c>
@@ -10870,9 +11255,9 @@
         <v>2.431</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="28"/>
-      <c r="B36" s="64"/>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" s="27"/>
+      <c r="B36" s="62"/>
       <c r="C36" s="26" t="s">
         <v>45</v>
       </c>
@@ -10892,9 +11277,9 @@
         <v>2.35</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="28"/>
-      <c r="B37" s="65"/>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" s="27"/>
+      <c r="B37" s="63"/>
       <c r="C37" s="26" t="s">
         <v>46</v>
       </c>
@@ -10914,9 +11299,9 @@
         <v>4.5430000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="28"/>
-      <c r="B38" s="63">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" s="27"/>
+      <c r="B38" s="61">
         <v>2</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -10932,9 +11317,9 @@
         <v>0.22600000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="28"/>
-      <c r="B39" s="64"/>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" s="27"/>
+      <c r="B39" s="62"/>
       <c r="C39" s="2" t="s">
         <v>44</v>
       </c>
@@ -10954,9 +11339,9 @@
         <v>2.2989999999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="28"/>
-      <c r="B40" s="64"/>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" s="27"/>
+      <c r="B40" s="62"/>
       <c r="C40" s="2" t="s">
         <v>45</v>
       </c>
@@ -10976,9 +11361,9 @@
         <v>2.3109999999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="28"/>
-      <c r="B41" s="65"/>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" s="27"/>
+      <c r="B41" s="63"/>
       <c r="C41" s="2" t="s">
         <v>46</v>
       </c>
@@ -10998,9 +11383,9 @@
         <v>4.5709999999999997</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="28"/>
-      <c r="B42" s="63">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" s="27"/>
+      <c r="B42" s="61">
         <v>3</v>
       </c>
       <c r="C42" s="26" t="s">
@@ -11016,9 +11401,9 @@
         <v>0.24199999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="28"/>
-      <c r="B43" s="64"/>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" s="27"/>
+      <c r="B43" s="62"/>
       <c r="C43" s="26" t="s">
         <v>44</v>
       </c>
@@ -11032,9 +11417,9 @@
         <v>0.78100000000000003</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="28"/>
-      <c r="B44" s="64"/>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" s="27"/>
+      <c r="B44" s="62"/>
       <c r="C44" s="26" t="s">
         <v>45</v>
       </c>
@@ -11054,9 +11439,9 @@
         <v>2.343</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="28"/>
-      <c r="B45" s="65"/>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" s="27"/>
+      <c r="B45" s="63"/>
       <c r="C45" s="26" t="s">
         <v>46</v>
       </c>
@@ -11076,9 +11461,9 @@
         <v>4.5750000000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="28"/>
-      <c r="B46" s="63">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" s="27"/>
+      <c r="B46" s="61">
         <v>4</v>
       </c>
       <c r="C46" s="2" t="s">
@@ -11094,9 +11479,9 @@
         <v>0.23799999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="28"/>
-      <c r="B47" s="64"/>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47" s="27"/>
+      <c r="B47" s="62"/>
       <c r="C47" s="2" t="s">
         <v>44</v>
       </c>
@@ -11110,9 +11495,9 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="28"/>
-      <c r="B48" s="64"/>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48" s="27"/>
+      <c r="B48" s="62"/>
       <c r="C48" s="2" t="s">
         <v>45</v>
       </c>
@@ -11126,9 +11511,9 @@
         <v>0.79700000000000004</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="28"/>
-      <c r="B49" s="65"/>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A49" s="27"/>
+      <c r="B49" s="63"/>
       <c r="C49" s="2" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
Finish testing with webcam
</commit_message>
<xml_diff>
--- a/detect_methods_comp.xlsx
+++ b/detect_methods_comp.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iwaya\Escritorio\Code\FaceRecogServer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369FED87-8541-4031-9F45-51113A03B670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3C5695-DBEE-4324-A17D-B7F9D8EB7965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25710" yWindow="1140" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resultados" sheetId="6" r:id="rId1"/>
-    <sheet name="Resize (OpenCV)" sheetId="2" r:id="rId2"/>
-    <sheet name="get_frontal_face_detector()" sheetId="1" r:id="rId3"/>
-    <sheet name="DeepNeuralNetworks Methods" sheetId="3" r:id="rId4"/>
-    <sheet name="Combinación métodos" sheetId="4" r:id="rId5"/>
-    <sheet name="Tiempos procesamiento" sheetId="5" r:id="rId6"/>
+    <sheet name="Resultados webcam Go1" sheetId="7" r:id="rId2"/>
+    <sheet name="Resize (OpenCV)" sheetId="2" r:id="rId3"/>
+    <sheet name="get_frontal_face_detector()" sheetId="1" r:id="rId4"/>
+    <sheet name="DeepNeuralNetworks Methods" sheetId="3" r:id="rId5"/>
+    <sheet name="Combinación métodos" sheetId="4" r:id="rId6"/>
+    <sheet name="Tiempos procesamiento" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="98">
   <si>
     <t>Up Sampling [dlib.get_frontal_face_detector()]</t>
   </si>
@@ -279,12 +280,69 @@
   <si>
     <t>El tamaño de la imagen es muy pequeño para realizar detección facial,  la tasa de transmisión no mejora (fps)</t>
   </si>
+  <si>
+    <t>0.37 - 0.39</t>
+  </si>
+  <si>
+    <t>10 - 10.3</t>
+  </si>
+  <si>
+    <t>0.37 - 0.40</t>
+  </si>
+  <si>
+    <t>0.37 - 0.41</t>
+  </si>
+  <si>
+    <t>0.44 - 0.51</t>
+  </si>
+  <si>
+    <t>0.45 - 0.51</t>
+  </si>
+  <si>
+    <t>10 - 10.4</t>
+  </si>
+  <si>
+    <t>2.5 metros</t>
+  </si>
+  <si>
+    <t>0.44 - 0.50</t>
+  </si>
+  <si>
+    <t>0.89 - 1.11</t>
+  </si>
+  <si>
+    <t>0.89 - 1.12</t>
+  </si>
+  <si>
+    <t>0.90 - 1.11</t>
+  </si>
+  <si>
+    <t>10 - 10.6</t>
+  </si>
+  <si>
+    <t>10 - 10.7</t>
+  </si>
+  <si>
+    <t>0.37 - 0.38</t>
+  </si>
+  <si>
+    <t>0.36 - 0.39</t>
+  </si>
+  <si>
+    <t>1.41 - 1.52</t>
+  </si>
+  <si>
+    <t>1.40 - 1.52</t>
+  </si>
+  <si>
+    <t>1.41 - 1.54</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,8 +358,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -365,6 +429,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -627,7 +703,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -707,19 +783,22 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -731,6 +810,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -740,22 +822,49 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -770,10 +879,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -788,25 +897,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -818,20 +909,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7948,58 +8036,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD554FA1-10E3-4A88-8A1D-54AF58A25FC5}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10:I13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" style="1" customWidth="1"/>
-    <col min="2" max="3" width="15.6328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="15.5703125" style="1" customWidth="1"/>
     <col min="4" max="5" width="17" style="1" customWidth="1"/>
-    <col min="6" max="6" width="29.453125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="32.54296875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.7265625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="41.54296875" style="66" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="32.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="67.5703125" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="67" t="s">
+    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="67" t="s">
+      <c r="E1" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="F1" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="67" t="s">
+      <c r="G1" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="67" t="s">
+      <c r="H1" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="65" t="s">
+      <c r="I1" s="27" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="27">
+    <row r="2" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="32">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="27">
+      <c r="C2" s="32">
         <v>9.3000000000000007</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -8017,14 +8105,14 @@
       <c r="H2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="I2" s="64" t="s">
+      <c r="I2" s="31" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
       <c r="D3" s="2" t="s">
         <v>51</v>
       </c>
@@ -8040,12 +8128,12 @@
       <c r="H3" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I3" s="64"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
+      <c r="I3" s="31"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
       <c r="D4" s="2" t="s">
         <v>52</v>
       </c>
@@ -8061,12 +8149,12 @@
       <c r="H4" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="64"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
+      <c r="I4" s="31"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="32"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
       <c r="D5" s="2" t="s">
         <v>53</v>
       </c>
@@ -8082,14 +8170,14 @@
       <c r="H5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I5" s="64"/>
-    </row>
-    <row r="6" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27" t="s">
+      <c r="I5" s="31"/>
+    </row>
+    <row r="6" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="32"/>
+      <c r="B6" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="32">
         <v>22.32</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -8107,14 +8195,14 @@
       <c r="H6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="I6" s="64" t="s">
+      <c r="I6" s="31" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
       <c r="D7" s="2" t="s">
         <v>51</v>
       </c>
@@ -8130,12 +8218,12 @@
       <c r="H7" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I7" s="64"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
+      <c r="I7" s="31"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
       <c r="D8" s="2" t="s">
         <v>52</v>
       </c>
@@ -8151,12 +8239,12 @@
       <c r="H8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="64"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
+      <c r="I8" s="31"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
       <c r="D9" s="2" t="s">
         <v>53</v>
       </c>
@@ -8172,14 +8260,14 @@
       <c r="H9" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I9" s="64"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27" t="s">
+      <c r="I9" s="31"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="32">
         <v>23.43</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -8197,14 +8285,14 @@
       <c r="H10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I10" s="64" t="s">
+      <c r="I10" s="31" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
       <c r="D11" s="2" t="s">
         <v>51</v>
       </c>
@@ -8220,12 +8308,12 @@
       <c r="H11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I11" s="64"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
+      <c r="I11" s="31"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
       <c r="D12" s="2" t="s">
         <v>52</v>
       </c>
@@ -8241,12 +8329,12 @@
       <c r="H12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I12" s="64"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
+      <c r="I12" s="31"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
       <c r="D13" s="2" t="s">
         <v>53</v>
       </c>
@@ -8262,14 +8350,14 @@
       <c r="H13" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I13" s="64"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27" t="s">
+      <c r="I13" s="31"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="32"/>
+      <c r="B14" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="C14" s="27">
+      <c r="C14" s="32">
         <v>23.42</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -8287,14 +8375,14 @@
       <c r="H14" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I14" s="64" t="s">
+      <c r="I14" s="31" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="32"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
       <c r="D15" s="2" t="s">
         <v>51</v>
       </c>
@@ -8310,12 +8398,12 @@
       <c r="H15" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I15" s="64"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="27"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
+      <c r="I15" s="31"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
       <c r="D16" s="2" t="s">
         <v>52</v>
       </c>
@@ -8331,12 +8419,12 @@
       <c r="H16" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I16" s="64"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
+      <c r="I16" s="31"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
       <c r="D17" s="2" t="s">
         <v>53</v>
       </c>
@@ -8352,14 +8440,14 @@
       <c r="H17" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I17" s="64"/>
-    </row>
-    <row r="18" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="27"/>
-      <c r="B18" s="27" t="s">
+      <c r="I17" s="31"/>
+    </row>
+    <row r="18" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="32"/>
+      <c r="B18" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="27">
+      <c r="C18" s="32">
         <v>24</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -8377,14 +8465,14 @@
       <c r="H18" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I18" s="64" t="s">
+      <c r="I18" s="31" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
       <c r="D19" s="2" t="s">
         <v>51</v>
       </c>
@@ -8400,12 +8488,12 @@
       <c r="H19" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I19" s="64"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="27"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
+      <c r="I19" s="31"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
       <c r="D20" s="2" t="s">
         <v>52</v>
       </c>
@@ -8421,12 +8509,12 @@
       <c r="H20" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I20" s="64"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="27"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
+      <c r="I20" s="31"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
       <c r="D21" s="2" t="s">
         <v>53</v>
       </c>
@@ -8442,14 +8530,14 @@
       <c r="H21" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="64"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="27"/>
-      <c r="B22" s="64" t="s">
+      <c r="I21" s="31"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="32"/>
+      <c r="B22" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="27">
+      <c r="C22" s="32">
         <v>23.43</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -8467,14 +8555,14 @@
       <c r="H22" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="I22" s="64" t="s">
+      <c r="I22" s="31" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="27"/>
-      <c r="B23" s="64"/>
-      <c r="C23" s="27"/>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="32"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="32"/>
       <c r="D23" s="2" t="s">
         <v>51</v>
       </c>
@@ -8490,12 +8578,12 @@
       <c r="H23" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I23" s="64"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="27"/>
-      <c r="B24" s="64"/>
-      <c r="C24" s="27"/>
+      <c r="I23" s="31"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="32"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="32"/>
       <c r="D24" s="2" t="s">
         <v>52</v>
       </c>
@@ -8511,12 +8599,12 @@
       <c r="H24" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I24" s="64"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="27"/>
-      <c r="B25" s="64"/>
-      <c r="C25" s="27"/>
+      <c r="I24" s="31"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="32"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="32"/>
       <c r="D25" s="2" t="s">
         <v>53</v>
       </c>
@@ -8532,10 +8620,11 @@
       <c r="H25" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I25" s="64"/>
+      <c r="I25" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C14:C17"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="C22:C25"/>
     <mergeCell ref="I22:I25"/>
@@ -8554,7 +8643,6 @@
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="C6:C9"/>
     <mergeCell ref="C10:C13"/>
-    <mergeCell ref="C14:C17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8562,6 +8650,223 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3643DA04-5652-4938-8036-B031F2BB2592}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="69" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="69" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="69" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="72">
+        <v>1</v>
+      </c>
+      <c r="B2" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="71" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="71" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="71" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="71" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="72"/>
+      <c r="B3" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="71" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="71" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="71" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="71" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="72"/>
+      <c r="B4" s="71" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="71" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="71" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="71" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" s="71" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="32">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="70" t="s">
+        <v>91</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="32"/>
+      <c r="B6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="70" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="32"/>
+      <c r="B7" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="70" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="72">
+        <v>3</v>
+      </c>
+      <c r="B8" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="71" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="71" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="71" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="72"/>
+      <c r="B9" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="71" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="71" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" s="71" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="72"/>
+      <c r="B10" s="71" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="71" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="71" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="F10" s="71" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6706964-F93E-4934-BEB2-8D6878ECF54C}">
   <dimension ref="A1:O8"/>
   <sheetViews>
@@ -8569,22 +8874,22 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="12" width="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>27</v>
       </c>
@@ -8612,7 +8917,7 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
@@ -8656,7 +8961,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -8704,7 +9009,7 @@
         <v>1.1792592592592592</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -8752,7 +9057,7 @@
         <v>3.2364197530864196</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -8800,7 +9105,7 @@
         <v>6.2976543209876548</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -8848,7 +9153,7 @@
         <v>10.856419753086421</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -8896,7 +9201,7 @@
         <v>16.636172839506173</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -8943,405 +9248,6 @@
         <f t="shared" si="1"/>
         <v>23.849876543209877</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q13"/>
-  <sheetViews>
-    <sheetView zoomScale="84" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="44.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="9.1796875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="5">
-        <v>37.4</v>
-      </c>
-      <c r="E3" s="5">
-        <f>D3/60</f>
-        <v>0.62333333333333329</v>
-      </c>
-      <c r="F3" s="8">
-        <f>D3/37</f>
-        <v>1.0108108108108107</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M3" s="5">
-        <v>98.11</v>
-      </c>
-      <c r="N3" s="5">
-        <f t="shared" ref="N3:N8" si="0">M3/60</f>
-        <v>1.6351666666666667</v>
-      </c>
-      <c r="O3" s="8">
-        <f>M3/81</f>
-        <v>1.2112345679012346</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="5">
-        <v>76.239999999999995</v>
-      </c>
-      <c r="E4" s="5">
-        <f t="shared" ref="E4:E8" si="1">D4/60</f>
-        <v>1.2706666666666666</v>
-      </c>
-      <c r="F4" s="8">
-        <f t="shared" ref="F4:F8" si="2">D4/37</f>
-        <v>2.0605405405405404</v>
-      </c>
-      <c r="H4" s="2">
-        <v>1</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M4" s="5">
-        <v>268.89999999999998</v>
-      </c>
-      <c r="N4" s="5">
-        <f t="shared" si="0"/>
-        <v>4.4816666666666665</v>
-      </c>
-      <c r="O4" s="8">
-        <f t="shared" ref="O4:O6" si="3">M4/81</f>
-        <v>3.3197530864197526</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" s="6">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="5">
-        <v>191.54</v>
-      </c>
-      <c r="E5" s="5">
-        <f t="shared" si="1"/>
-        <v>3.192333333333333</v>
-      </c>
-      <c r="F5" s="8">
-        <f t="shared" si="2"/>
-        <v>5.1767567567567569</v>
-      </c>
-      <c r="H5" s="2">
-        <v>2</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M5" s="5">
-        <v>956.49</v>
-      </c>
-      <c r="N5" s="5">
-        <f t="shared" si="0"/>
-        <v>15.9415</v>
-      </c>
-      <c r="O5" s="8">
-        <f t="shared" si="3"/>
-        <v>11.808518518518518</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="5">
-        <v>419.84</v>
-      </c>
-      <c r="E6" s="5">
-        <f t="shared" si="1"/>
-        <v>6.9973333333333327</v>
-      </c>
-      <c r="F6" s="8">
-        <f t="shared" si="2"/>
-        <v>11.347027027027027</v>
-      </c>
-      <c r="H6" s="2">
-        <v>3</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M6" s="5">
-        <v>3674.01</v>
-      </c>
-      <c r="N6" s="5">
-        <f t="shared" si="0"/>
-        <v>61.233500000000006</v>
-      </c>
-      <c r="O6" s="8">
-        <f t="shared" si="3"/>
-        <v>45.358148148148153</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A7" s="7">
-        <v>4</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="5">
-        <v>1559.89</v>
-      </c>
-      <c r="E7" s="5">
-        <f t="shared" si="1"/>
-        <v>25.99816666666667</v>
-      </c>
-      <c r="F7" s="8">
-        <f t="shared" si="2"/>
-        <v>42.159189189189192</v>
-      </c>
-      <c r="H7" s="2">
-        <v>4</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M7" s="5">
-        <v>14483.55</v>
-      </c>
-      <c r="N7" s="5">
-        <f t="shared" si="0"/>
-        <v>241.39249999999998</v>
-      </c>
-      <c r="O7" s="8">
-        <f>M7/81</f>
-        <v>178.80925925925925</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" s="6">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="5">
-        <v>5878.92</v>
-      </c>
-      <c r="E8" s="5">
-        <f t="shared" si="1"/>
-        <v>97.981999999999999</v>
-      </c>
-      <c r="F8" s="8">
-        <f t="shared" si="2"/>
-        <v>158.88972972972974</v>
-      </c>
-      <c r="H8" s="2">
-        <v>5</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M8" s="5">
-        <v>59016.9</v>
-      </c>
-      <c r="N8" s="5">
-        <f t="shared" si="0"/>
-        <v>983.61500000000001</v>
-      </c>
-      <c r="O8" s="8">
-        <f>M8/81</f>
-        <v>728.60370370370367</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9351,30 +9257,31 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EDFC79-1BF5-4D0E-ADD4-A69D2D4846CD}">
-  <dimension ref="A1:O5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView zoomScale="92" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView zoomScale="84" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" customWidth="1"/>
-    <col min="7" max="7" width="11.54296875" customWidth="1"/>
-    <col min="8" max="8" width="42.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="4.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>27</v>
       </c>
@@ -9387,24 +9294,16 @@
       <c r="D1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
       <c r="H1" s="10" t="s">
         <v>28</v>
       </c>
       <c r="I1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>5</v>
@@ -9418,12 +9317,11 @@
       <c r="E2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="11"/>
       <c r="H2" s="13" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="I2" s="13" t="s">
         <v>17</v>
@@ -9443,34 +9341,33 @@
       <c r="N2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="21" t="s">
+      <c r="O2" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
-        <v>13</v>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" s="5">
-        <v>152.66999999999999</v>
+        <v>37.4</v>
       </c>
       <c r="E3" s="5">
         <f>D3/60</f>
-        <v>2.5444999999999998</v>
+        <v>0.62333333333333329</v>
       </c>
       <c r="F3" s="8">
         <f>D3/37</f>
-        <v>4.1262162162162159</v>
-      </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="6" t="s">
-        <v>13</v>
+        <v>1.0108108108108107</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>1</v>
@@ -9479,47 +9376,46 @@
         <v>1</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M3" s="2">
-        <v>1305.19</v>
+        <v>1</v>
+      </c>
+      <c r="M3" s="5">
+        <v>98.11</v>
       </c>
       <c r="N3" s="5">
-        <f>M3/60</f>
-        <v>21.753166666666669</v>
+        <f t="shared" ref="N3:N8" si="0">M3/60</f>
+        <v>1.6351666666666667</v>
       </c>
       <c r="O3" s="8">
         <f>M3/81</f>
-        <v>16.113456790123458</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="4" t="s">
+        <v>1.2112345679012346</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
         <v>1</v>
       </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="D4" s="5">
-        <v>152.69</v>
+        <v>76.239999999999995</v>
       </c>
       <c r="E4" s="5">
-        <f t="shared" ref="E4:E5" si="0">D4/60</f>
-        <v>2.5448333333333335</v>
+        <f t="shared" ref="E4:E8" si="1">D4/60</f>
+        <v>1.2706666666666666</v>
       </c>
       <c r="F4" s="8">
-        <f t="shared" ref="F4:F5" si="1">D4/37</f>
-        <v>4.1267567567567571</v>
-      </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="6" t="s">
-        <v>14</v>
+        <f t="shared" ref="F4:F8" si="2">D4/37</f>
+        <v>2.0605405405405404</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>1</v>
@@ -9528,26 +9424,26 @@
         <v>1</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M4" s="2">
-        <v>1674.66</v>
+        <v>1</v>
+      </c>
+      <c r="M4" s="5">
+        <v>268.89999999999998</v>
       </c>
       <c r="N4" s="5">
-        <f>M4/60</f>
-        <v>27.911000000000001</v>
+        <f t="shared" si="0"/>
+        <v>4.4816666666666665</v>
       </c>
       <c r="O4" s="8">
-        <f t="shared" ref="O4:O5" si="2">M4/81</f>
-        <v>20.674814814814816</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
-        <v>15</v>
+        <f t="shared" ref="O4:O6" si="3">M4/81</f>
+        <v>3.3197530864197526</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -9556,25 +9452,24 @@
         <v>1</v>
       </c>
       <c r="D5" s="5">
-        <v>1212.56</v>
+        <v>191.54</v>
       </c>
       <c r="E5" s="5">
-        <f t="shared" si="0"/>
-        <v>20.209333333333333</v>
+        <f t="shared" si="1"/>
+        <v>3.192333333333333</v>
       </c>
       <c r="F5" s="8">
-        <f t="shared" si="1"/>
-        <v>32.77189189189189</v>
-      </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="6" t="s">
-        <v>15</v>
+        <f t="shared" si="2"/>
+        <v>5.1767567567567569</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>4</v>
@@ -9583,16 +9478,175 @@
         <v>4</v>
       </c>
       <c r="M5" s="5">
-        <v>12024.66</v>
+        <v>956.49</v>
       </c>
       <c r="N5" s="5">
-        <f>M5/60</f>
-        <v>200.411</v>
+        <f t="shared" si="0"/>
+        <v>15.9415</v>
       </c>
       <c r="O5" s="8">
+        <f t="shared" si="3"/>
+        <v>11.808518518518518</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="5">
+        <v>419.84</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" si="1"/>
+        <v>6.9973333333333327</v>
+      </c>
+      <c r="F6" s="8">
         <f t="shared" si="2"/>
-        <v>148.45259259259259</v>
-      </c>
+        <v>11.347027027027027</v>
+      </c>
+      <c r="H6" s="2">
+        <v>3</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="5">
+        <v>3674.01</v>
+      </c>
+      <c r="N6" s="5">
+        <f t="shared" si="0"/>
+        <v>61.233500000000006</v>
+      </c>
+      <c r="O6" s="8">
+        <f t="shared" si="3"/>
+        <v>45.358148148148153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1559.89</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="1"/>
+        <v>25.99816666666667</v>
+      </c>
+      <c r="F7" s="8">
+        <f t="shared" si="2"/>
+        <v>42.159189189189192</v>
+      </c>
+      <c r="H7" s="2">
+        <v>4</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M7" s="5">
+        <v>14483.55</v>
+      </c>
+      <c r="N7" s="5">
+        <f t="shared" si="0"/>
+        <v>241.39249999999998</v>
+      </c>
+      <c r="O7" s="8">
+        <f>M7/81</f>
+        <v>178.80925925925925</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="5">
+        <v>5878.92</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="1"/>
+        <v>97.981999999999999</v>
+      </c>
+      <c r="F8" s="8">
+        <f t="shared" si="2"/>
+        <v>158.88972972972974</v>
+      </c>
+      <c r="H8" s="2">
+        <v>5</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M8" s="5">
+        <v>59016.9</v>
+      </c>
+      <c r="N8" s="5">
+        <f t="shared" si="0"/>
+        <v>983.61500000000001</v>
+      </c>
+      <c r="O8" s="8">
+        <f>M8/81</f>
+        <v>728.60370370370367</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9602,6 +9656,257 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43EDFC79-1BF5-4D0E-ADD4-A69D2D4846CD}">
+  <dimension ref="A1:O5"/>
+  <sheetViews>
+    <sheetView zoomScale="92" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="11"/>
+      <c r="H2" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
+        <v>152.66999999999999</v>
+      </c>
+      <c r="E3" s="5">
+        <f>D3/60</f>
+        <v>2.5444999999999998</v>
+      </c>
+      <c r="F3" s="8">
+        <f>D3/37</f>
+        <v>4.1262162162162159</v>
+      </c>
+      <c r="G3" s="12"/>
+      <c r="H3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="2">
+        <v>1305.19</v>
+      </c>
+      <c r="N3" s="5">
+        <f>M3/60</f>
+        <v>21.753166666666669</v>
+      </c>
+      <c r="O3" s="8">
+        <f>M3/81</f>
+        <v>16.113456790123458</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
+        <v>152.69</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" ref="E4:E5" si="0">D4/60</f>
+        <v>2.5448333333333335</v>
+      </c>
+      <c r="F4" s="8">
+        <f t="shared" ref="F4:F5" si="1">D4/37</f>
+        <v>4.1267567567567571</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" s="2">
+        <v>1674.66</v>
+      </c>
+      <c r="N4" s="5">
+        <f>M4/60</f>
+        <v>27.911000000000001</v>
+      </c>
+      <c r="O4" s="8">
+        <f t="shared" ref="O4:O5" si="2">M4/81</f>
+        <v>20.674814814814816</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1212.56</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" si="0"/>
+        <v>20.209333333333333</v>
+      </c>
+      <c r="F5" s="8">
+        <f t="shared" si="1"/>
+        <v>32.77189189189189</v>
+      </c>
+      <c r="G5" s="12"/>
+      <c r="H5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" s="5">
+        <v>12024.66</v>
+      </c>
+      <c r="N5" s="5">
+        <f>M5/60</f>
+        <v>200.411</v>
+      </c>
+      <c r="O5" s="8">
+        <f t="shared" si="2"/>
+        <v>148.45259259259259</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB5E59B-51C7-438E-AB32-5EE19B87C996}">
   <dimension ref="A1:J49"/>
   <sheetViews>
@@ -9609,999 +9914,1008 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7265625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7265625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.81640625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="8.54296875" style="14" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="14" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="14" customWidth="1"/>
     <col min="8" max="8" width="15" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.54296875" style="14" customWidth="1"/>
-    <col min="10" max="10" width="9.1796875" style="14" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" style="14" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="56"/>
+      <c r="C1" s="47"/>
       <c r="D1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="56"/>
+      <c r="F1" s="47"/>
       <c r="G1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="H1" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="56"/>
+      <c r="I1" s="47"/>
       <c r="J1" s="25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="16">
         <v>1.2</v>
       </c>
-      <c r="C2" s="49">
+      <c r="C2" s="52">
         <v>1</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="49" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="16">
         <v>1.5</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="49">
+      <c r="I2" s="52">
         <v>1</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="33" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="29"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="50"/>
       <c r="B3" s="15">
         <v>1.5</v>
       </c>
       <c r="C3" s="43"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="29"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="50"/>
       <c r="F3" s="15">
         <v>2</v>
       </c>
-      <c r="G3" s="33"/>
-      <c r="H3" s="29"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="50"/>
       <c r="I3" s="43"/>
-      <c r="J3" s="33"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="29"/>
+      <c r="J3" s="34"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="50"/>
       <c r="B4" s="15">
         <v>1.7</v>
       </c>
       <c r="C4" s="43"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="29"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="50"/>
       <c r="F4" s="15">
         <v>2.5</v>
       </c>
-      <c r="G4" s="33"/>
-      <c r="H4" s="29"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="50"/>
       <c r="I4" s="43">
         <v>2</v>
       </c>
-      <c r="J4" s="33"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="29"/>
+      <c r="J4" s="34"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="50"/>
       <c r="B5" s="15">
         <v>2</v>
       </c>
       <c r="C5" s="43"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="29"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="50"/>
       <c r="F5" s="15">
         <v>3</v>
       </c>
-      <c r="G5" s="33"/>
-      <c r="H5" s="29"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="50"/>
       <c r="I5" s="43"/>
-      <c r="J5" s="33"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="29"/>
+      <c r="J5" s="34"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="50"/>
       <c r="B6" s="15">
         <v>2.5</v>
       </c>
       <c r="C6" s="43"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="42" t="s">
+      <c r="D6" s="34"/>
+      <c r="E6" s="51" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="15">
         <v>1.5</v>
       </c>
-      <c r="G6" s="33"/>
-      <c r="H6" s="42" t="s">
+      <c r="G6" s="34"/>
+      <c r="H6" s="51" t="s">
         <v>14</v>
       </c>
       <c r="I6" s="43">
         <v>1</v>
       </c>
-      <c r="J6" s="33"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="29"/>
+      <c r="J6" s="34"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="50"/>
       <c r="B7" s="15">
         <v>3</v>
       </c>
       <c r="C7" s="43"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="42"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="51"/>
       <c r="F7" s="15">
         <v>2</v>
       </c>
-      <c r="G7" s="33"/>
-      <c r="H7" s="42"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="51"/>
       <c r="I7" s="43"/>
-      <c r="J7" s="33"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="29"/>
+      <c r="J7" s="34"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="50"/>
       <c r="B8" s="15">
         <v>1.2</v>
       </c>
       <c r="C8" s="43">
         <v>2</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="42"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="51"/>
       <c r="F8" s="15">
         <v>2.5</v>
       </c>
-      <c r="G8" s="33"/>
-      <c r="H8" s="42"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="51"/>
       <c r="I8" s="43">
         <v>2</v>
       </c>
-      <c r="J8" s="33"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="29"/>
+      <c r="J8" s="34"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="50"/>
       <c r="B9" s="15">
         <v>1.5</v>
       </c>
       <c r="C9" s="43"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="42"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="51"/>
       <c r="F9" s="15">
         <v>3</v>
       </c>
-      <c r="G9" s="33"/>
-      <c r="H9" s="42"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="51"/>
       <c r="I9" s="43"/>
-      <c r="J9" s="33"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="29"/>
+      <c r="J9" s="34"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="50"/>
       <c r="B10" s="15">
         <v>1.7</v>
       </c>
       <c r="C10" s="43"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="42" t="s">
+      <c r="D10" s="34"/>
+      <c r="E10" s="51" t="s">
         <v>15</v>
       </c>
       <c r="F10" s="15">
         <v>1.5</v>
       </c>
-      <c r="G10" s="33"/>
-      <c r="H10" s="42" t="s">
+      <c r="G10" s="34"/>
+      <c r="H10" s="51" t="s">
         <v>15</v>
       </c>
       <c r="I10" s="43">
         <v>1</v>
       </c>
-      <c r="J10" s="33"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="29"/>
+      <c r="J10" s="34"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="50"/>
       <c r="B11" s="15">
         <v>2</v>
       </c>
       <c r="C11" s="43"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="42"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="51"/>
       <c r="F11" s="15">
         <v>2</v>
       </c>
-      <c r="G11" s="33"/>
-      <c r="H11" s="42"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="51"/>
       <c r="I11" s="43"/>
-      <c r="J11" s="33"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="29"/>
+      <c r="J11" s="34"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="50"/>
       <c r="B12" s="15">
         <v>2.5</v>
       </c>
       <c r="C12" s="43"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="42"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="51"/>
       <c r="F12" s="15">
         <v>2.5</v>
       </c>
-      <c r="G12" s="33"/>
-      <c r="H12" s="42"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="51"/>
       <c r="I12" s="43">
         <v>2</v>
       </c>
-      <c r="J12" s="33"/>
-    </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="30"/>
+      <c r="J12" s="34"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="53"/>
       <c r="B13" s="17">
         <v>3</v>
       </c>
-      <c r="C13" s="54"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="55"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="54"/>
       <c r="F13" s="17">
         <v>3</v>
       </c>
-      <c r="G13" s="34"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="34"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="44" t="s">
+      <c r="G13" s="35"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="35"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="55" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="18">
         <v>1.2</v>
       </c>
-      <c r="C14" s="47">
+      <c r="C14" s="58">
         <v>1</v>
       </c>
-      <c r="D14" s="35" t="s">
+      <c r="D14" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="44" t="s">
+      <c r="E14" s="55" t="s">
         <v>13</v>
       </c>
       <c r="F14" s="18">
         <v>1.5</v>
       </c>
-      <c r="G14" s="32" t="s">
+      <c r="G14" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="H14" s="44" t="s">
+      <c r="H14" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="47">
+      <c r="I14" s="58">
         <v>1</v>
       </c>
-      <c r="J14" s="32" t="s">
+      <c r="J14" s="33" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="45"/>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="56"/>
       <c r="B15" s="2">
         <v>1.5</v>
       </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="45"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="56"/>
       <c r="F15" s="2">
         <v>2</v>
       </c>
-      <c r="G15" s="33"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="33"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="45"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="34"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="56"/>
       <c r="B16" s="2">
         <v>1.7</v>
       </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="45"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="56"/>
       <c r="F16" s="2">
         <v>2.5</v>
       </c>
-      <c r="G16" s="33"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="27">
+      <c r="G16" s="34"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="32">
         <v>2</v>
       </c>
-      <c r="J16" s="33"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="45"/>
+      <c r="J16" s="34"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="56"/>
       <c r="B17" s="2">
         <v>2</v>
       </c>
-      <c r="C17" s="27"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="45"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="56"/>
       <c r="F17" s="2">
         <v>3</v>
       </c>
-      <c r="G17" s="33"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="33"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="45"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="56"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="34"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="56"/>
       <c r="B18" s="2">
         <v>2.5</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="38" t="s">
+      <c r="C18" s="32"/>
+      <c r="D18" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="41" t="s">
+      <c r="E18" s="59" t="s">
         <v>14</v>
       </c>
       <c r="F18" s="2">
         <v>1.5</v>
       </c>
-      <c r="G18" s="33"/>
-      <c r="H18" s="41" t="s">
+      <c r="G18" s="34"/>
+      <c r="H18" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="I18" s="27">
+      <c r="I18" s="32">
         <v>1</v>
       </c>
-      <c r="J18" s="33"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="45"/>
+      <c r="J18" s="34"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="56"/>
       <c r="B19" s="2">
         <v>3</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="41"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="59"/>
       <c r="F19" s="2">
         <v>2</v>
       </c>
-      <c r="G19" s="33"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="33"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="45"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="34"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="56"/>
       <c r="B20" s="2">
         <v>1.2</v>
       </c>
-      <c r="C20" s="27">
+      <c r="C20" s="32">
         <v>2</v>
       </c>
       <c r="D20" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="41"/>
+      <c r="E20" s="59"/>
       <c r="F20" s="2">
         <v>2.5</v>
       </c>
-      <c r="G20" s="33"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="27">
+      <c r="G20" s="34"/>
+      <c r="H20" s="59"/>
+      <c r="I20" s="32">
         <v>2</v>
       </c>
-      <c r="J20" s="33"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" s="45"/>
+      <c r="J20" s="34"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="56"/>
       <c r="B21" s="2">
         <v>1.5</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="38" t="s">
+      <c r="C21" s="32"/>
+      <c r="D21" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="41"/>
+      <c r="E21" s="59"/>
       <c r="F21" s="2">
         <v>3</v>
       </c>
-      <c r="G21" s="33"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="33"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="45"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="34"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="56"/>
       <c r="B22" s="2">
         <v>1.7</v>
       </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="41" t="s">
+      <c r="C22" s="32"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="59" t="s">
         <v>15</v>
       </c>
       <c r="F22" s="2">
         <v>1.5</v>
       </c>
-      <c r="G22" s="33"/>
-      <c r="H22" s="41" t="s">
+      <c r="G22" s="34"/>
+      <c r="H22" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="I22" s="27">
+      <c r="I22" s="32">
         <v>1</v>
       </c>
-      <c r="J22" s="33"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="45"/>
+      <c r="J22" s="34"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="56"/>
       <c r="B23" s="2">
         <v>2</v>
       </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="41"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="59"/>
       <c r="F23" s="2">
         <v>2</v>
       </c>
-      <c r="G23" s="33"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="33"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" s="45"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="34"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="56"/>
       <c r="B24" s="2">
         <v>2.5</v>
       </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="41"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="59"/>
       <c r="F24" s="2">
         <v>2.5</v>
       </c>
-      <c r="G24" s="33"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="27">
+      <c r="G24" s="34"/>
+      <c r="H24" s="59"/>
+      <c r="I24" s="32">
         <v>2</v>
       </c>
-      <c r="J24" s="33"/>
-    </row>
-    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="46"/>
+      <c r="J24" s="34"/>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="57"/>
       <c r="B25" s="20">
         <v>3</v>
       </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="48"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="60"/>
       <c r="F25" s="20">
         <v>3</v>
       </c>
-      <c r="G25" s="34"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="34"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A26" s="28" t="s">
+      <c r="G25" s="35"/>
+      <c r="H25" s="60"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="35"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="49" t="s">
         <v>18</v>
       </c>
       <c r="B26" s="16">
         <v>1.2</v>
       </c>
-      <c r="C26" s="49">
+      <c r="C26" s="52">
         <v>1</v>
       </c>
-      <c r="D26" s="35" t="s">
+      <c r="D26" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="28" t="s">
+      <c r="E26" s="49" t="s">
         <v>13</v>
       </c>
       <c r="F26" s="16">
         <v>1.5</v>
       </c>
-      <c r="G26" s="35" t="s">
+      <c r="G26" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="H26" s="50" t="s">
+      <c r="H26" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="I26" s="52">
+      <c r="I26" s="63">
         <v>1</v>
       </c>
-      <c r="J26" s="32" t="s">
+      <c r="J26" s="33" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A27" s="29"/>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="50"/>
       <c r="B27" s="15">
         <v>1.5</v>
       </c>
       <c r="C27" s="43"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="29"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="50"/>
       <c r="F27" s="15">
         <v>2</v>
       </c>
-      <c r="G27" s="36"/>
-      <c r="H27" s="51"/>
-      <c r="I27" s="53"/>
-      <c r="J27" s="33"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A28" s="29"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="62"/>
+      <c r="I27" s="64"/>
+      <c r="J27" s="34"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="50"/>
       <c r="B28" s="15">
         <v>1.7</v>
       </c>
       <c r="C28" s="43"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="29"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="50"/>
       <c r="F28" s="15">
         <v>2.5</v>
       </c>
-      <c r="G28" s="36"/>
-      <c r="H28" s="51"/>
-      <c r="I28" s="53">
+      <c r="G28" s="38"/>
+      <c r="H28" s="62"/>
+      <c r="I28" s="64">
         <v>2</v>
       </c>
-      <c r="J28" s="33"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A29" s="29"/>
+      <c r="J28" s="34"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="50"/>
       <c r="B29" s="15">
         <v>2</v>
       </c>
       <c r="C29" s="43"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="29"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="50"/>
       <c r="F29" s="15">
         <v>3</v>
       </c>
-      <c r="G29" s="36"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="53"/>
-      <c r="J29" s="33"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A30" s="29"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="62"/>
+      <c r="I29" s="64"/>
+      <c r="J29" s="34"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="50"/>
       <c r="B30" s="15">
         <v>2.5</v>
       </c>
       <c r="C30" s="43"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="42" t="s">
+      <c r="D30" s="38"/>
+      <c r="E30" s="51" t="s">
         <v>14</v>
       </c>
       <c r="F30" s="15">
         <v>1.5</v>
       </c>
-      <c r="G30" s="37"/>
-      <c r="H30" s="42" t="s">
+      <c r="G30" s="39"/>
+      <c r="H30" s="51" t="s">
         <v>14</v>
       </c>
       <c r="I30" s="43">
         <v>1</v>
       </c>
-      <c r="J30" s="33"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A31" s="29"/>
+      <c r="J30" s="34"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="50"/>
       <c r="B31" s="15">
         <v>3</v>
       </c>
       <c r="C31" s="43"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="42"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="51"/>
       <c r="F31" s="15">
         <v>2</v>
       </c>
       <c r="G31" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="H31" s="42"/>
+      <c r="H31" s="51"/>
       <c r="I31" s="43"/>
-      <c r="J31" s="33"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A32" s="29"/>
+      <c r="J31" s="34"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="50"/>
       <c r="B32" s="15">
         <v>1.2</v>
       </c>
       <c r="C32" s="43">
         <v>2</v>
       </c>
-      <c r="D32" s="36"/>
-      <c r="E32" s="42"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="51"/>
       <c r="F32" s="15">
         <v>2.5</v>
       </c>
-      <c r="G32" s="58" t="s">
+      <c r="G32" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="H32" s="42"/>
+      <c r="H32" s="51"/>
       <c r="I32" s="43">
         <v>2</v>
       </c>
-      <c r="J32" s="33"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A33" s="29"/>
+      <c r="J32" s="34"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="50"/>
       <c r="B33" s="15">
         <v>1.5</v>
       </c>
       <c r="C33" s="43"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="42"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="51"/>
       <c r="F33" s="15">
         <v>3</v>
       </c>
-      <c r="G33" s="36"/>
-      <c r="H33" s="42"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="51"/>
       <c r="I33" s="43"/>
-      <c r="J33" s="33"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A34" s="29"/>
+      <c r="J33" s="34"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="50"/>
       <c r="B34" s="15">
         <v>1.7</v>
       </c>
       <c r="C34" s="43"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="42" t="s">
+      <c r="D34" s="38"/>
+      <c r="E34" s="51" t="s">
         <v>15</v>
       </c>
       <c r="F34" s="15">
         <v>1.5</v>
       </c>
-      <c r="G34" s="36"/>
-      <c r="H34" s="42" t="s">
+      <c r="G34" s="38"/>
+      <c r="H34" s="51" t="s">
         <v>15</v>
       </c>
       <c r="I34" s="43">
         <v>1</v>
       </c>
-      <c r="J34" s="33"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A35" s="29"/>
+      <c r="J34" s="34"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="50"/>
       <c r="B35" s="15">
         <v>2</v>
       </c>
       <c r="C35" s="43"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="42"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="51"/>
       <c r="F35" s="15">
         <v>2</v>
       </c>
-      <c r="G35" s="36"/>
-      <c r="H35" s="42"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="51"/>
       <c r="I35" s="43"/>
-      <c r="J35" s="39"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A36" s="29"/>
+      <c r="J35" s="36"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="50"/>
       <c r="B36" s="15">
         <v>2.5</v>
       </c>
       <c r="C36" s="43"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="42"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="51"/>
       <c r="F36" s="15">
         <v>2.5</v>
       </c>
-      <c r="G36" s="36"/>
-      <c r="H36" s="42"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="51"/>
       <c r="I36" s="43">
         <v>2</v>
       </c>
-      <c r="J36" s="59" t="s">
+      <c r="J36" s="45" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="30"/>
+    <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="53"/>
       <c r="B37" s="17">
         <v>3</v>
       </c>
-      <c r="C37" s="54"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="55"/>
+      <c r="C37" s="44"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="54"/>
       <c r="F37" s="17">
         <v>3</v>
       </c>
-      <c r="G37" s="40"/>
-      <c r="H37" s="55"/>
-      <c r="I37" s="54"/>
-      <c r="J37" s="60"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A38" s="44" t="s">
+      <c r="G37" s="41"/>
+      <c r="H37" s="54"/>
+      <c r="I37" s="44"/>
+      <c r="J37" s="46"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="55" t="s">
         <v>17</v>
       </c>
       <c r="B38" s="18">
         <v>1.2</v>
       </c>
-      <c r="C38" s="47">
+      <c r="C38" s="58">
         <v>1</v>
       </c>
-      <c r="D38" s="35" t="s">
+      <c r="D38" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="44" t="s">
+      <c r="E38" s="55" t="s">
         <v>13</v>
       </c>
       <c r="F38" s="18">
         <v>1.5</v>
       </c>
-      <c r="G38" s="35" t="s">
+      <c r="G38" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="H38" s="44" t="s">
+      <c r="H38" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="I38" s="47">
+      <c r="I38" s="58">
         <v>1</v>
       </c>
-      <c r="J38" s="35" t="s">
+      <c r="J38" s="37" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A39" s="45"/>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="56"/>
       <c r="B39" s="2">
         <v>1.5</v>
       </c>
-      <c r="C39" s="27"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="45"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="56"/>
       <c r="F39" s="2">
         <v>2</v>
       </c>
-      <c r="G39" s="36"/>
-      <c r="H39" s="45"/>
-      <c r="I39" s="27"/>
-      <c r="J39" s="36"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A40" s="45"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="56"/>
+      <c r="I39" s="32"/>
+      <c r="J39" s="38"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="56"/>
       <c r="B40" s="2">
         <v>1.7</v>
       </c>
-      <c r="C40" s="27"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="45"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="56"/>
       <c r="F40" s="2">
         <v>2.5</v>
       </c>
-      <c r="G40" s="36"/>
-      <c r="H40" s="45"/>
-      <c r="I40" s="27">
+      <c r="G40" s="38"/>
+      <c r="H40" s="56"/>
+      <c r="I40" s="32">
         <v>2</v>
       </c>
-      <c r="J40" s="36"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A41" s="45"/>
+      <c r="J40" s="38"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="56"/>
       <c r="B41" s="2">
         <v>2</v>
       </c>
-      <c r="C41" s="27"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="45"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="56"/>
       <c r="F41" s="2">
         <v>3</v>
       </c>
-      <c r="G41" s="36"/>
-      <c r="H41" s="45"/>
-      <c r="I41" s="27"/>
-      <c r="J41" s="36"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A42" s="45"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="56"/>
+      <c r="I41" s="32"/>
+      <c r="J41" s="38"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="56"/>
       <c r="B42" s="2">
         <v>2.5</v>
       </c>
-      <c r="C42" s="27"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="41" t="s">
+      <c r="C42" s="32"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="59" t="s">
         <v>14</v>
       </c>
       <c r="F42" s="2">
         <v>1.5</v>
       </c>
-      <c r="G42" s="36"/>
-      <c r="H42" s="41" t="s">
+      <c r="G42" s="38"/>
+      <c r="H42" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="I42" s="27">
+      <c r="I42" s="32">
         <v>1</v>
       </c>
-      <c r="J42" s="36"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A43" s="45"/>
+      <c r="J42" s="38"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="56"/>
       <c r="B43" s="2">
         <v>3</v>
       </c>
-      <c r="C43" s="27"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="41"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="59"/>
       <c r="F43" s="2">
         <v>2</v>
       </c>
-      <c r="G43" s="36"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="36"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A44" s="45"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="59"/>
+      <c r="I43" s="32"/>
+      <c r="J43" s="38"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="56"/>
       <c r="B44" s="2">
         <v>1.2</v>
       </c>
-      <c r="C44" s="27">
+      <c r="C44" s="32">
         <v>2</v>
       </c>
-      <c r="D44" s="36"/>
-      <c r="E44" s="41"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="59"/>
       <c r="F44" s="2">
         <v>2.5</v>
       </c>
-      <c r="G44" s="36"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="27">
+      <c r="G44" s="38"/>
+      <c r="H44" s="59"/>
+      <c r="I44" s="32">
         <v>2</v>
       </c>
-      <c r="J44" s="36"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A45" s="45"/>
+      <c r="J44" s="38"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="56"/>
       <c r="B45" s="2">
         <v>1.5</v>
       </c>
-      <c r="C45" s="27"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="41"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="59"/>
       <c r="F45" s="2">
         <v>3</v>
       </c>
-      <c r="G45" s="36"/>
-      <c r="H45" s="41"/>
-      <c r="I45" s="27"/>
-      <c r="J45" s="36"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A46" s="45"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="59"/>
+      <c r="I45" s="32"/>
+      <c r="J45" s="38"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="56"/>
       <c r="B46" s="2">
         <v>1.7</v>
       </c>
-      <c r="C46" s="27"/>
-      <c r="D46" s="36"/>
-      <c r="E46" s="41" t="s">
+      <c r="C46" s="32"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="59" t="s">
         <v>15</v>
       </c>
       <c r="F46" s="2">
         <v>1.5</v>
       </c>
-      <c r="G46" s="36"/>
-      <c r="H46" s="41" t="s">
+      <c r="G46" s="38"/>
+      <c r="H46" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="I46" s="27">
+      <c r="I46" s="32">
         <v>1</v>
       </c>
-      <c r="J46" s="36"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A47" s="45"/>
+      <c r="J46" s="38"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="56"/>
       <c r="B47" s="2">
         <v>2</v>
       </c>
-      <c r="C47" s="27"/>
-      <c r="D47" s="36"/>
-      <c r="E47" s="41"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="38"/>
+      <c r="E47" s="59"/>
       <c r="F47" s="2">
         <v>2</v>
       </c>
-      <c r="G47" s="36"/>
-      <c r="H47" s="41"/>
-      <c r="I47" s="27"/>
-      <c r="J47" s="36"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A48" s="45"/>
+      <c r="G47" s="38"/>
+      <c r="H47" s="59"/>
+      <c r="I47" s="32"/>
+      <c r="J47" s="38"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="56"/>
       <c r="B48" s="2">
         <v>2.5</v>
       </c>
-      <c r="C48" s="27"/>
-      <c r="D48" s="36"/>
-      <c r="E48" s="41"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="38"/>
+      <c r="E48" s="59"/>
       <c r="F48" s="2">
         <v>2.5</v>
       </c>
-      <c r="G48" s="36"/>
-      <c r="H48" s="41"/>
-      <c r="I48" s="27">
+      <c r="G48" s="38"/>
+      <c r="H48" s="59"/>
+      <c r="I48" s="32">
         <v>2</v>
       </c>
-      <c r="J48" s="36"/>
-    </row>
-    <row r="49" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="46"/>
+      <c r="J48" s="38"/>
+    </row>
+    <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="57"/>
       <c r="B49" s="20">
         <v>3</v>
       </c>
-      <c r="C49" s="31"/>
-      <c r="D49" s="40"/>
-      <c r="E49" s="48"/>
+      <c r="C49" s="42"/>
+      <c r="D49" s="41"/>
+      <c r="E49" s="60"/>
       <c r="F49" s="20">
         <v>3</v>
       </c>
-      <c r="G49" s="40"/>
-      <c r="H49" s="48"/>
-      <c r="I49" s="31"/>
-      <c r="J49" s="40"/>
+      <c r="G49" s="41"/>
+      <c r="H49" s="60"/>
+      <c r="I49" s="42"/>
+      <c r="J49" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="J14:J25"/>
-    <mergeCell ref="J26:J35"/>
-    <mergeCell ref="G26:G30"/>
-    <mergeCell ref="G32:G37"/>
-    <mergeCell ref="J38:J49"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="I36:I37"/>
-    <mergeCell ref="J36:J37"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="G2:G13"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="C8:C13"/>
-    <mergeCell ref="C2:C7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="H6:H9"/>
-    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="I48:I49"/>
+    <mergeCell ref="D2:D13"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D21:D25"/>
+    <mergeCell ref="D26:D37"/>
+    <mergeCell ref="E42:E45"/>
+    <mergeCell ref="H42:H45"/>
+    <mergeCell ref="I42:I43"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="G38:G49"/>
+    <mergeCell ref="D38:D49"/>
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="C38:C43"/>
+    <mergeCell ref="E38:E41"/>
+    <mergeCell ref="H38:H41"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="I40:I41"/>
+    <mergeCell ref="C44:C49"/>
+    <mergeCell ref="I44:I45"/>
+    <mergeCell ref="E46:E49"/>
+    <mergeCell ref="H46:H49"/>
+    <mergeCell ref="I46:I47"/>
+    <mergeCell ref="C26:C31"/>
+    <mergeCell ref="E26:E29"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="C32:C37"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="E34:E37"/>
+    <mergeCell ref="H34:H37"/>
+    <mergeCell ref="I34:I35"/>
     <mergeCell ref="J2:J13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="C14:C19"/>
@@ -10618,48 +10932,39 @@
     <mergeCell ref="E22:E25"/>
     <mergeCell ref="H22:H25"/>
     <mergeCell ref="I22:I23"/>
-    <mergeCell ref="C26:C31"/>
-    <mergeCell ref="E26:E29"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="E30:E33"/>
-    <mergeCell ref="C32:C37"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="E34:E37"/>
-    <mergeCell ref="H34:H37"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="H38:H41"/>
-    <mergeCell ref="I38:I39"/>
-    <mergeCell ref="I40:I41"/>
-    <mergeCell ref="C44:C49"/>
-    <mergeCell ref="I44:I45"/>
-    <mergeCell ref="E46:E49"/>
-    <mergeCell ref="H46:H49"/>
-    <mergeCell ref="I46:I47"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="I48:I49"/>
-    <mergeCell ref="D2:D13"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="D21:D25"/>
-    <mergeCell ref="D26:D37"/>
-    <mergeCell ref="E42:E45"/>
-    <mergeCell ref="H42:H45"/>
-    <mergeCell ref="I42:I43"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="G38:G49"/>
-    <mergeCell ref="D38:D49"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="C38:C43"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="C8:C13"/>
+    <mergeCell ref="C2:C7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="H10:H13"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="G2:G13"/>
+    <mergeCell ref="J14:J25"/>
+    <mergeCell ref="J26:J35"/>
+    <mergeCell ref="G26:G30"/>
+    <mergeCell ref="G32:G37"/>
+    <mergeCell ref="J38:J49"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="I36:I37"/>
+    <mergeCell ref="J36:J37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E5ED226-BA1A-41A1-A969-1FDD4768045A}">
   <dimension ref="A1:H49"/>
   <sheetViews>
@@ -10667,19 +10972,19 @@
       <selection activeCell="C39" sqref="C39:G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="1"/>
     <col min="4" max="4" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.54296875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7265625" style="1"/>
+    <col min="5" max="5" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>32</v>
       </c>
@@ -10705,11 +11010,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="27" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="61">
+      <c r="B2" s="66">
         <v>1</v>
       </c>
       <c r="C2" s="26">
@@ -10725,9 +11030,9 @@
         <v>7.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="27"/>
-      <c r="B3" s="62"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="32"/>
+      <c r="B3" s="67"/>
       <c r="C3" s="26">
         <v>2</v>
       </c>
@@ -10747,9 +11052,9 @@
         <v>2.1970000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="27"/>
-      <c r="B4" s="62"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="32"/>
+      <c r="B4" s="67"/>
       <c r="C4" s="26">
         <v>3</v>
       </c>
@@ -10769,9 +11074,9 @@
         <v>3.1779999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="27"/>
-      <c r="B5" s="63"/>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="32"/>
+      <c r="B5" s="68"/>
       <c r="C5" s="26">
         <v>4</v>
       </c>
@@ -10791,9 +11096,9 @@
         <v>7.1150000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="27"/>
-      <c r="B6" s="61">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="32"/>
+      <c r="B6" s="66">
         <v>2</v>
       </c>
       <c r="C6" s="2">
@@ -10809,9 +11114,9 @@
         <v>5.8000000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="27"/>
-      <c r="B7" s="62"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="32"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="2">
         <v>2</v>
       </c>
@@ -10825,9 +11130,9 @@
         <v>0.184</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="27"/>
-      <c r="B8" s="62"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="32"/>
+      <c r="B8" s="67"/>
       <c r="C8" s="2">
         <v>3</v>
       </c>
@@ -10847,9 +11152,9 @@
         <v>2.302</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="27"/>
-      <c r="B9" s="63"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="32"/>
+      <c r="B9" s="68"/>
       <c r="C9" s="2">
         <v>4</v>
       </c>
@@ -10869,9 +11174,9 @@
         <v>4.5579999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="27"/>
-      <c r="B10" s="61">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
+      <c r="B10" s="66">
         <v>3</v>
       </c>
       <c r="C10" s="26">
@@ -10887,9 +11192,9 @@
         <v>6.3E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="27"/>
-      <c r="B11" s="62"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="32"/>
+      <c r="B11" s="67"/>
       <c r="C11" s="26">
         <v>2</v>
       </c>
@@ -10903,9 +11208,9 @@
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="27"/>
-      <c r="B12" s="62"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="32"/>
+      <c r="B12" s="67"/>
       <c r="C12" s="26">
         <v>3</v>
       </c>
@@ -10919,9 +11224,9 @@
         <v>0.73899999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="27"/>
-      <c r="B13" s="63"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="32"/>
+      <c r="B13" s="68"/>
       <c r="C13" s="26">
         <v>4</v>
       </c>
@@ -10935,9 +11240,9 @@
         <v>3.0089999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="27"/>
-      <c r="B14" s="61">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="32"/>
+      <c r="B14" s="66">
         <v>4</v>
       </c>
       <c r="C14" s="2">
@@ -10953,9 +11258,9 @@
         <v>5.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="27"/>
-      <c r="B15" s="62"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="32"/>
+      <c r="B15" s="67"/>
       <c r="C15" s="2">
         <v>2</v>
       </c>
@@ -10969,9 +11274,9 @@
         <v>0.184</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="27"/>
-      <c r="B16" s="62"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="32"/>
+      <c r="B16" s="67"/>
       <c r="C16" s="2">
         <v>3</v>
       </c>
@@ -10985,9 +11290,9 @@
         <v>0.76300000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="27"/>
-      <c r="B17" s="63"/>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="32"/>
+      <c r="B17" s="68"/>
       <c r="C17" s="2">
         <v>4</v>
       </c>
@@ -11001,11 +11306,11 @@
         <v>3.016</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="27" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="61">
+      <c r="B18" s="66">
         <v>1</v>
       </c>
       <c r="C18" s="26" t="s">
@@ -11027,9 +11332,9 @@
         <v>1.9159999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="27"/>
-      <c r="B19" s="62"/>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="32"/>
+      <c r="B19" s="67"/>
       <c r="C19" s="26"/>
       <c r="D19" s="26"/>
       <c r="E19" s="26"/>
@@ -11037,9 +11342,9 @@
       <c r="G19" s="26"/>
       <c r="H19" s="26"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="27"/>
-      <c r="B20" s="62"/>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="32"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
       <c r="E20" s="26"/>
@@ -11047,9 +11352,9 @@
       <c r="G20" s="26"/>
       <c r="H20" s="26"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="27"/>
-      <c r="B21" s="63"/>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="32"/>
+      <c r="B21" s="68"/>
       <c r="C21" s="26"/>
       <c r="D21" s="26"/>
       <c r="E21" s="26"/>
@@ -11057,9 +11362,9 @@
       <c r="G21" s="26"/>
       <c r="H21" s="26"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="27"/>
-      <c r="B22" s="61">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="32"/>
+      <c r="B22" s="66">
         <v>2</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -11081,9 +11386,9 @@
         <v>1.9139999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="27"/>
-      <c r="B23" s="62"/>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="32"/>
+      <c r="B23" s="67"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -11091,9 +11396,9 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="27"/>
-      <c r="B24" s="62"/>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="32"/>
+      <c r="B24" s="67"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -11101,9 +11406,9 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="27"/>
-      <c r="B25" s="63"/>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="32"/>
+      <c r="B25" s="68"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -11111,9 +11416,9 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="27"/>
-      <c r="B26" s="61">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="32"/>
+      <c r="B26" s="66">
         <v>3</v>
       </c>
       <c r="C26" s="26" t="s">
@@ -11129,9 +11434,9 @@
         <v>0.39600000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="27"/>
-      <c r="B27" s="62"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="32"/>
+      <c r="B27" s="67"/>
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
       <c r="E27" s="26"/>
@@ -11139,9 +11444,9 @@
       <c r="G27" s="26"/>
       <c r="H27" s="26"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="27"/>
-      <c r="B28" s="62"/>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="32"/>
+      <c r="B28" s="67"/>
       <c r="C28" s="26"/>
       <c r="D28" s="26"/>
       <c r="E28" s="26"/>
@@ -11149,9 +11454,9 @@
       <c r="G28" s="26"/>
       <c r="H28" s="26"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="27"/>
-      <c r="B29" s="63"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="32"/>
+      <c r="B29" s="68"/>
       <c r="C29" s="26"/>
       <c r="D29" s="26"/>
       <c r="E29" s="26"/>
@@ -11159,9 +11464,9 @@
       <c r="G29" s="26"/>
       <c r="H29" s="26"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="27"/>
-      <c r="B30" s="61">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="32"/>
+      <c r="B30" s="66">
         <v>4</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -11177,9 +11482,9 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="27"/>
-      <c r="B31" s="62"/>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="32"/>
+      <c r="B31" s="67"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -11187,9 +11492,9 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="27"/>
-      <c r="B32" s="62"/>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="32"/>
+      <c r="B32" s="67"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -11197,9 +11502,9 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="27"/>
-      <c r="B33" s="63"/>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="32"/>
+      <c r="B33" s="68"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -11207,11 +11512,11 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="27" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="61">
+      <c r="B34" s="66">
         <v>1</v>
       </c>
       <c r="C34" s="26" t="s">
@@ -11233,9 +11538,9 @@
         <v>1.732</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="27"/>
-      <c r="B35" s="62"/>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="32"/>
+      <c r="B35" s="67"/>
       <c r="C35" s="26" t="s">
         <v>44</v>
       </c>
@@ -11255,9 +11560,9 @@
         <v>2.431</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="27"/>
-      <c r="B36" s="62"/>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="32"/>
+      <c r="B36" s="67"/>
       <c r="C36" s="26" t="s">
         <v>45</v>
       </c>
@@ -11277,9 +11582,9 @@
         <v>2.35</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" s="27"/>
-      <c r="B37" s="63"/>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="32"/>
+      <c r="B37" s="68"/>
       <c r="C37" s="26" t="s">
         <v>46</v>
       </c>
@@ -11299,9 +11604,9 @@
         <v>4.5430000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A38" s="27"/>
-      <c r="B38" s="61">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="32"/>
+      <c r="B38" s="66">
         <v>2</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -11317,9 +11622,9 @@
         <v>0.22600000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" s="27"/>
-      <c r="B39" s="62"/>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="32"/>
+      <c r="B39" s="67"/>
       <c r="C39" s="2" t="s">
         <v>44</v>
       </c>
@@ -11339,9 +11644,9 @@
         <v>2.2989999999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A40" s="27"/>
-      <c r="B40" s="62"/>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="32"/>
+      <c r="B40" s="67"/>
       <c r="C40" s="2" t="s">
         <v>45</v>
       </c>
@@ -11361,9 +11666,9 @@
         <v>2.3109999999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A41" s="27"/>
-      <c r="B41" s="63"/>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="32"/>
+      <c r="B41" s="68"/>
       <c r="C41" s="2" t="s">
         <v>46</v>
       </c>
@@ -11383,9 +11688,9 @@
         <v>4.5709999999999997</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A42" s="27"/>
-      <c r="B42" s="61">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="32"/>
+      <c r="B42" s="66">
         <v>3</v>
       </c>
       <c r="C42" s="26" t="s">
@@ -11401,9 +11706,9 @@
         <v>0.24199999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A43" s="27"/>
-      <c r="B43" s="62"/>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="32"/>
+      <c r="B43" s="67"/>
       <c r="C43" s="26" t="s">
         <v>44</v>
       </c>
@@ -11417,9 +11722,9 @@
         <v>0.78100000000000003</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A44" s="27"/>
-      <c r="B44" s="62"/>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="32"/>
+      <c r="B44" s="67"/>
       <c r="C44" s="26" t="s">
         <v>45</v>
       </c>
@@ -11439,9 +11744,9 @@
         <v>2.343</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A45" s="27"/>
-      <c r="B45" s="63"/>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="32"/>
+      <c r="B45" s="68"/>
       <c r="C45" s="26" t="s">
         <v>46</v>
       </c>
@@ -11461,9 +11766,9 @@
         <v>4.5750000000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A46" s="27"/>
-      <c r="B46" s="61">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="32"/>
+      <c r="B46" s="66">
         <v>4</v>
       </c>
       <c r="C46" s="2" t="s">
@@ -11479,9 +11784,9 @@
         <v>0.23799999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A47" s="27"/>
-      <c r="B47" s="62"/>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="32"/>
+      <c r="B47" s="67"/>
       <c r="C47" s="2" t="s">
         <v>44</v>
       </c>
@@ -11495,9 +11800,9 @@
         <v>0.80400000000000005</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A48" s="27"/>
-      <c r="B48" s="62"/>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="32"/>
+      <c r="B48" s="67"/>
       <c r="C48" s="2" t="s">
         <v>45</v>
       </c>
@@ -11511,9 +11816,9 @@
         <v>0.79700000000000004</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A49" s="27"/>
-      <c r="B49" s="63"/>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="32"/>
+      <c r="B49" s="68"/>
       <c r="C49" s="2" t="s">
         <v>46</v>
       </c>
@@ -11529,6 +11834,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B17"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="B42:B45"/>
     <mergeCell ref="B46:B49"/>
@@ -11539,11 +11849,6 @@
     <mergeCell ref="B34:B37"/>
     <mergeCell ref="B38:B41"/>
     <mergeCell ref="B22:B25"/>
-    <mergeCell ref="A2:A17"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>